<commit_message>
🐞 Use precinct id, not polling center on reports (#1729)
Parent issue: https://github.com/sequentech/meta/issues/6339
</commit_message>
<xml_diff>
--- a/packages/windmill/external-bin/janitor/extra_files-2025-02-19.xlsx
+++ b/packages/windmill/external-bin/janitor/extra_files-2025-02-19.xlsx
@@ -18,7 +18,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1450" uniqueCount="687">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1451" uniqueCount="686">
   <si>
     <t>name</t>
   </si>
@@ -233,7 +233,7 @@
     <t>Manually verify voter</t>
   </si>
   <si>
-    <t>SBEI|OFOV</t>
+    <t>OFOV</t>
   </si>
   <si>
     <t>OVCS_EVENTS</t>
@@ -1759,9 +1759,6 @@
   </si>
   <si>
     <t>ofov</t>
-  </si>
-  <si>
-    <t>OFOV</t>
   </si>
   <si>
     <t>permissions</t>
@@ -28987,7 +28984,7 @@
         <v>486</v>
       </c>
       <c r="B3" s="34" t="s">
-        <v>487</v>
+        <v>34</v>
       </c>
       <c r="C3" s="43" t="b">
         <v>1</v>
@@ -35909,25 +35906,25 @@
   <sheetData>
     <row r="1" ht="15.75" customHeight="1">
       <c r="A1" s="45" t="s">
-        <v>488</v>
+        <v>487</v>
       </c>
       <c r="B1" s="46" t="s">
         <v>439</v>
       </c>
       <c r="C1" s="46" t="s">
-        <v>489</v>
+        <v>488</v>
       </c>
       <c r="D1" s="46" t="s">
         <v>486</v>
       </c>
       <c r="E1" s="47" t="s">
+        <v>489</v>
+      </c>
+      <c r="F1" s="47" t="s">
         <v>490</v>
       </c>
-      <c r="F1" s="47" t="s">
+      <c r="G1" s="47" t="s">
         <v>491</v>
-      </c>
-      <c r="G1" s="47" t="s">
-        <v>492</v>
       </c>
       <c r="H1" s="48"/>
       <c r="I1" s="48"/>
@@ -35951,19 +35948,19 @@
     </row>
     <row r="2" ht="15.75" customHeight="1">
       <c r="A2" s="50" t="s">
+        <v>492</v>
+      </c>
+      <c r="B2" s="51" t="s">
         <v>493</v>
       </c>
-      <c r="B2" s="51" t="s">
-        <v>494</v>
-      </c>
       <c r="C2" s="52" t="s">
-        <v>494</v>
+        <v>493</v>
       </c>
       <c r="D2" s="42"/>
       <c r="E2" s="53"/>
       <c r="F2" s="54"/>
       <c r="G2" s="52" t="s">
-        <v>494</v>
+        <v>493</v>
       </c>
       <c r="H2" s="54"/>
       <c r="I2" s="54"/>
@@ -35987,21 +35984,21 @@
     </row>
     <row r="3" ht="15.75" customHeight="1">
       <c r="A3" s="50" t="s">
-        <v>495</v>
+        <v>494</v>
       </c>
       <c r="B3" s="52" t="s">
-        <v>494</v>
+        <v>493</v>
       </c>
       <c r="C3" s="52" t="s">
-        <v>494</v>
+        <v>493</v>
       </c>
       <c r="D3" s="52" t="s">
-        <v>494</v>
+        <v>493</v>
       </c>
       <c r="E3" s="41"/>
       <c r="F3" s="41"/>
       <c r="G3" s="52" t="s">
-        <v>494</v>
+        <v>493</v>
       </c>
       <c r="H3" s="41"/>
       <c r="I3" s="41"/>
@@ -36025,14 +36022,14 @@
     </row>
     <row r="4" ht="15.75" customHeight="1">
       <c r="A4" s="50" t="s">
-        <v>496</v>
+        <v>495</v>
       </c>
       <c r="B4" s="52" t="s">
-        <v>494</v>
+        <v>493</v>
       </c>
       <c r="C4" s="41"/>
       <c r="D4" s="52" t="s">
-        <v>494</v>
+        <v>493</v>
       </c>
       <c r="E4" s="41"/>
       <c r="F4" s="41"/>
@@ -36059,22 +36056,22 @@
     </row>
     <row r="5" ht="15.75" customHeight="1">
       <c r="A5" s="50" t="s">
-        <v>497</v>
+        <v>496</v>
       </c>
       <c r="B5" s="52" t="s">
-        <v>494</v>
+        <v>493</v>
       </c>
       <c r="C5" s="52" t="s">
-        <v>494</v>
+        <v>493</v>
       </c>
       <c r="D5" s="52" t="s">
-        <v>494</v>
+        <v>493</v>
       </c>
       <c r="E5" s="52" t="s">
-        <v>494</v>
+        <v>493</v>
       </c>
       <c r="F5" s="52" t="s">
-        <v>494</v>
+        <v>493</v>
       </c>
       <c r="G5" s="41"/>
       <c r="H5" s="41"/>
@@ -36099,14 +36096,14 @@
     </row>
     <row r="6" ht="15.75" customHeight="1">
       <c r="A6" s="50" t="s">
-        <v>498</v>
+        <v>497</v>
       </c>
       <c r="B6" s="52" t="s">
-        <v>494</v>
+        <v>493</v>
       </c>
       <c r="C6" s="41"/>
       <c r="D6" s="52" t="s">
-        <v>494</v>
+        <v>493</v>
       </c>
       <c r="E6" s="41"/>
       <c r="F6" s="41"/>
@@ -36133,10 +36130,10 @@
     </row>
     <row r="7" ht="15.75" customHeight="1">
       <c r="A7" s="50" t="s">
-        <v>499</v>
+        <v>498</v>
       </c>
       <c r="B7" s="52" t="s">
-        <v>494</v>
+        <v>493</v>
       </c>
       <c r="C7" s="42"/>
       <c r="D7" s="41"/>
@@ -36165,14 +36162,14 @@
     </row>
     <row r="8" ht="15.75" customHeight="1">
       <c r="A8" s="50" t="s">
-        <v>500</v>
+        <v>499</v>
       </c>
       <c r="B8" s="52" t="s">
-        <v>494</v>
+        <v>493</v>
       </c>
       <c r="C8" s="41"/>
       <c r="D8" s="52" t="s">
-        <v>494</v>
+        <v>493</v>
       </c>
       <c r="E8" s="41"/>
       <c r="F8" s="41"/>
@@ -36199,16 +36196,16 @@
     </row>
     <row r="9" ht="15.75" customHeight="1">
       <c r="A9" s="50" t="s">
-        <v>501</v>
+        <v>500</v>
       </c>
       <c r="B9" s="52" t="s">
-        <v>494</v>
+        <v>493</v>
       </c>
       <c r="C9" s="52" t="s">
-        <v>494</v>
+        <v>493</v>
       </c>
       <c r="D9" s="52" t="s">
-        <v>494</v>
+        <v>493</v>
       </c>
       <c r="E9" s="41"/>
       <c r="F9" s="41"/>
@@ -36235,10 +36232,10 @@
     </row>
     <row r="10" ht="15.75" customHeight="1">
       <c r="A10" s="50" t="s">
-        <v>502</v>
+        <v>501</v>
       </c>
       <c r="B10" s="52" t="s">
-        <v>494</v>
+        <v>493</v>
       </c>
       <c r="C10" s="41"/>
       <c r="D10" s="41"/>
@@ -36267,10 +36264,10 @@
     </row>
     <row r="11" ht="15.75" customHeight="1">
       <c r="A11" s="50" t="s">
-        <v>503</v>
+        <v>502</v>
       </c>
       <c r="B11" s="52" t="s">
-        <v>494</v>
+        <v>493</v>
       </c>
       <c r="C11" s="41"/>
       <c r="D11" s="41"/>
@@ -36299,14 +36296,14 @@
     </row>
     <row r="12" ht="15.75" customHeight="1">
       <c r="A12" s="50" t="s">
-        <v>504</v>
+        <v>503</v>
       </c>
       <c r="B12" s="52" t="s">
-        <v>494</v>
+        <v>493</v>
       </c>
       <c r="C12" s="42"/>
       <c r="D12" s="52" t="s">
-        <v>494</v>
+        <v>493</v>
       </c>
       <c r="E12" s="41"/>
       <c r="F12" s="41"/>
@@ -36333,10 +36330,10 @@
     </row>
     <row r="13" ht="15.75" customHeight="1">
       <c r="A13" s="50" t="s">
-        <v>505</v>
+        <v>504</v>
       </c>
       <c r="B13" s="52" t="s">
-        <v>494</v>
+        <v>493</v>
       </c>
       <c r="C13" s="41"/>
       <c r="D13" s="41"/>
@@ -36365,21 +36362,21 @@
     </row>
     <row r="14" ht="15.75" customHeight="1">
       <c r="A14" s="50" t="s">
-        <v>506</v>
+        <v>505</v>
       </c>
       <c r="B14" s="52" t="s">
-        <v>494</v>
+        <v>493</v>
       </c>
       <c r="C14" s="52" t="s">
-        <v>494</v>
+        <v>493</v>
       </c>
       <c r="D14" s="52" t="s">
-        <v>494</v>
+        <v>493</v>
       </c>
       <c r="E14" s="41"/>
       <c r="F14" s="41"/>
       <c r="G14" s="52" t="s">
-        <v>494</v>
+        <v>493</v>
       </c>
       <c r="H14" s="41"/>
       <c r="I14" s="41"/>
@@ -36403,10 +36400,10 @@
     </row>
     <row r="15" ht="15.75" customHeight="1">
       <c r="A15" s="50" t="s">
-        <v>507</v>
+        <v>506</v>
       </c>
       <c r="B15" s="52" t="s">
-        <v>494</v>
+        <v>493</v>
       </c>
       <c r="C15" s="41"/>
       <c r="D15" s="41"/>
@@ -36435,17 +36432,17 @@
     </row>
     <row r="16" ht="15.75" customHeight="1">
       <c r="A16" s="50" t="s">
-        <v>508</v>
+        <v>507</v>
       </c>
       <c r="B16" s="52" t="s">
-        <v>494</v>
+        <v>493</v>
       </c>
       <c r="C16" s="42"/>
       <c r="D16" s="41"/>
       <c r="E16" s="41"/>
       <c r="F16" s="41"/>
       <c r="G16" s="52" t="s">
-        <v>494</v>
+        <v>493</v>
       </c>
       <c r="H16" s="41"/>
       <c r="I16" s="41"/>
@@ -36469,10 +36466,10 @@
     </row>
     <row r="17" ht="15.75" customHeight="1">
       <c r="A17" s="50" t="s">
-        <v>509</v>
+        <v>508</v>
       </c>
       <c r="B17" s="52" t="s">
-        <v>494</v>
+        <v>493</v>
       </c>
       <c r="C17" s="42"/>
       <c r="D17" s="41"/>
@@ -36501,10 +36498,10 @@
     </row>
     <row r="18" ht="15.75" customHeight="1">
       <c r="A18" s="50" t="s">
-        <v>510</v>
+        <v>509</v>
       </c>
       <c r="B18" s="52" t="s">
-        <v>494</v>
+        <v>493</v>
       </c>
       <c r="C18" s="41"/>
       <c r="D18" s="41"/>
@@ -36533,10 +36530,10 @@
     </row>
     <row r="19" ht="15.75" customHeight="1">
       <c r="A19" s="50" t="s">
-        <v>511</v>
+        <v>510</v>
       </c>
       <c r="B19" s="52" t="s">
-        <v>494</v>
+        <v>493</v>
       </c>
       <c r="C19" s="42"/>
       <c r="D19" s="42"/>
@@ -36565,10 +36562,10 @@
     </row>
     <row r="20" ht="15.75" customHeight="1">
       <c r="A20" s="50" t="s">
-        <v>512</v>
+        <v>511</v>
       </c>
       <c r="B20" s="52" t="s">
-        <v>494</v>
+        <v>493</v>
       </c>
       <c r="C20" s="41"/>
       <c r="D20" s="41"/>
@@ -36597,21 +36594,21 @@
     </row>
     <row r="21" ht="15.75" customHeight="1">
       <c r="A21" s="50" t="s">
-        <v>513</v>
+        <v>512</v>
       </c>
       <c r="B21" s="52" t="s">
-        <v>494</v>
+        <v>493</v>
       </c>
       <c r="C21" s="52" t="s">
-        <v>494</v>
+        <v>493</v>
       </c>
       <c r="D21" s="52" t="s">
-        <v>494</v>
+        <v>493</v>
       </c>
       <c r="E21" s="41"/>
       <c r="F21" s="41"/>
       <c r="G21" s="52" t="s">
-        <v>494</v>
+        <v>493</v>
       </c>
       <c r="H21" s="41"/>
       <c r="I21" s="41"/>
@@ -36635,10 +36632,10 @@
     </row>
     <row r="22" ht="15.75" customHeight="1">
       <c r="A22" s="50" t="s">
-        <v>514</v>
+        <v>513</v>
       </c>
       <c r="B22" s="52" t="s">
-        <v>494</v>
+        <v>493</v>
       </c>
       <c r="C22" s="41"/>
       <c r="D22" s="41"/>
@@ -36667,14 +36664,14 @@
     </row>
     <row r="23" ht="15.75" customHeight="1">
       <c r="A23" s="50" t="s">
-        <v>515</v>
+        <v>514</v>
       </c>
       <c r="B23" s="52" t="s">
-        <v>494</v>
+        <v>493</v>
       </c>
       <c r="C23" s="41"/>
       <c r="D23" s="52" t="s">
-        <v>494</v>
+        <v>493</v>
       </c>
       <c r="E23" s="41"/>
       <c r="F23" s="41"/>
@@ -36701,21 +36698,21 @@
     </row>
     <row r="24" ht="15.75" customHeight="1">
       <c r="A24" s="50" t="s">
-        <v>516</v>
+        <v>515</v>
       </c>
       <c r="B24" s="52" t="s">
-        <v>494</v>
+        <v>493</v>
       </c>
       <c r="C24" s="52" t="s">
-        <v>494</v>
+        <v>493</v>
       </c>
       <c r="D24" s="52" t="s">
-        <v>494</v>
+        <v>493</v>
       </c>
       <c r="E24" s="41"/>
       <c r="F24" s="41"/>
       <c r="G24" s="52" t="s">
-        <v>494</v>
+        <v>493</v>
       </c>
       <c r="H24" s="41"/>
       <c r="I24" s="41"/>
@@ -36739,21 +36736,21 @@
     </row>
     <row r="25" ht="15.75" customHeight="1">
       <c r="A25" s="50" t="s">
-        <v>517</v>
+        <v>516</v>
       </c>
       <c r="B25" s="52" t="s">
-        <v>494</v>
+        <v>493</v>
       </c>
       <c r="C25" s="52" t="s">
-        <v>494</v>
+        <v>493</v>
       </c>
       <c r="D25" s="52" t="s">
-        <v>494</v>
+        <v>493</v>
       </c>
       <c r="E25" s="41"/>
       <c r="F25" s="41"/>
       <c r="G25" s="52" t="s">
-        <v>494</v>
+        <v>493</v>
       </c>
       <c r="H25" s="41"/>
       <c r="I25" s="41"/>
@@ -36777,17 +36774,17 @@
     </row>
     <row r="26" ht="15.75" customHeight="1">
       <c r="A26" s="50" t="s">
-        <v>518</v>
+        <v>517</v>
       </c>
       <c r="B26" s="52" t="s">
-        <v>494</v>
+        <v>493</v>
       </c>
       <c r="C26" s="41"/>
       <c r="D26" s="41"/>
       <c r="E26" s="41"/>
       <c r="F26" s="41"/>
       <c r="G26" s="52" t="s">
-        <v>494</v>
+        <v>493</v>
       </c>
       <c r="H26" s="41"/>
       <c r="I26" s="41"/>
@@ -36811,10 +36808,10 @@
     </row>
     <row r="27" ht="15.75" customHeight="1">
       <c r="A27" s="50" t="s">
-        <v>519</v>
+        <v>518</v>
       </c>
       <c r="B27" s="52" t="s">
-        <v>494</v>
+        <v>493</v>
       </c>
       <c r="C27" s="41"/>
       <c r="D27" s="41"/>
@@ -36843,13 +36840,13 @@
     </row>
     <row r="28" ht="15.75" customHeight="1">
       <c r="A28" s="50" t="s">
-        <v>520</v>
+        <v>519</v>
       </c>
       <c r="B28" s="52" t="s">
-        <v>494</v>
+        <v>493</v>
       </c>
       <c r="C28" s="52" t="s">
-        <v>494</v>
+        <v>493</v>
       </c>
       <c r="D28" s="42"/>
       <c r="E28" s="41"/>
@@ -36877,10 +36874,10 @@
     </row>
     <row r="29" ht="15.75" customHeight="1">
       <c r="A29" s="50" t="s">
-        <v>521</v>
+        <v>520</v>
       </c>
       <c r="B29" s="52" t="s">
-        <v>494</v>
+        <v>493</v>
       </c>
       <c r="C29" s="41"/>
       <c r="D29" s="41"/>
@@ -36909,13 +36906,13 @@
     </row>
     <row r="30" ht="15.75" customHeight="1">
       <c r="A30" s="50" t="s">
-        <v>522</v>
+        <v>521</v>
       </c>
       <c r="B30" s="52" t="s">
-        <v>494</v>
+        <v>493</v>
       </c>
       <c r="C30" s="52" t="s">
-        <v>494</v>
+        <v>493</v>
       </c>
       <c r="D30" s="41"/>
       <c r="E30" s="41"/>
@@ -36943,17 +36940,17 @@
     </row>
     <row r="31" ht="15.75" customHeight="1">
       <c r="A31" s="50" t="s">
-        <v>523</v>
+        <v>522</v>
       </c>
       <c r="B31" s="52" t="s">
-        <v>494</v>
+        <v>493</v>
       </c>
       <c r="C31" s="41"/>
       <c r="D31" s="41"/>
       <c r="E31" s="41"/>
       <c r="F31" s="41"/>
       <c r="G31" s="52" t="s">
-        <v>494</v>
+        <v>493</v>
       </c>
       <c r="H31" s="41"/>
       <c r="I31" s="41"/>
@@ -36977,25 +36974,25 @@
     </row>
     <row r="32" ht="15.75" customHeight="1">
       <c r="A32" s="50" t="s">
-        <v>524</v>
+        <v>523</v>
       </c>
       <c r="B32" s="52" t="s">
-        <v>494</v>
+        <v>493</v>
       </c>
       <c r="C32" s="52" t="s">
-        <v>494</v>
+        <v>493</v>
       </c>
       <c r="D32" s="52" t="s">
-        <v>494</v>
+        <v>493</v>
       </c>
       <c r="E32" s="52" t="s">
-        <v>494</v>
+        <v>493</v>
       </c>
       <c r="F32" s="52" t="s">
-        <v>494</v>
+        <v>493</v>
       </c>
       <c r="G32" s="52" t="s">
-        <v>494</v>
+        <v>493</v>
       </c>
       <c r="H32" s="41"/>
       <c r="I32" s="41"/>
@@ -37019,21 +37016,23 @@
     </row>
     <row r="33" ht="15.75" customHeight="1">
       <c r="A33" s="50" t="s">
-        <v>525</v>
+        <v>524</v>
       </c>
       <c r="B33" s="52" t="s">
-        <v>494</v>
+        <v>493</v>
       </c>
       <c r="C33" s="52" t="s">
-        <v>494</v>
-      </c>
-      <c r="D33" s="41"/>
+        <v>493</v>
+      </c>
+      <c r="D33" s="52" t="s">
+        <v>493</v>
+      </c>
       <c r="E33" s="52" t="s">
-        <v>494</v>
+        <v>493</v>
       </c>
       <c r="F33" s="41"/>
       <c r="G33" s="52" t="s">
-        <v>494</v>
+        <v>493</v>
       </c>
       <c r="H33" s="41"/>
       <c r="I33" s="41"/>
@@ -37057,21 +37056,21 @@
     </row>
     <row r="34" ht="15.75" customHeight="1">
       <c r="A34" s="50" t="s">
-        <v>526</v>
+        <v>525</v>
       </c>
       <c r="B34" s="52" t="s">
-        <v>494</v>
+        <v>493</v>
       </c>
       <c r="C34" s="52" t="s">
-        <v>494</v>
+        <v>493</v>
       </c>
       <c r="D34" s="41"/>
       <c r="E34" s="52" t="s">
-        <v>494</v>
+        <v>493</v>
       </c>
       <c r="F34" s="41"/>
       <c r="G34" s="52" t="s">
-        <v>494</v>
+        <v>493</v>
       </c>
       <c r="H34" s="41"/>
       <c r="I34" s="41"/>
@@ -37095,23 +37094,23 @@
     </row>
     <row r="35" ht="15.75" customHeight="1">
       <c r="A35" s="50" t="s">
-        <v>527</v>
+        <v>526</v>
       </c>
       <c r="B35" s="52" t="s">
-        <v>494</v>
+        <v>493</v>
       </c>
       <c r="C35" s="52" t="s">
-        <v>494</v>
+        <v>493</v>
       </c>
       <c r="D35" s="52" t="s">
-        <v>494</v>
+        <v>493</v>
       </c>
       <c r="E35" s="52" t="s">
-        <v>494</v>
+        <v>493</v>
       </c>
       <c r="F35" s="41"/>
       <c r="G35" s="52" t="s">
-        <v>494</v>
+        <v>493</v>
       </c>
       <c r="H35" s="41"/>
       <c r="I35" s="41"/>
@@ -37135,19 +37134,19 @@
     </row>
     <row r="36" ht="15.75" customHeight="1">
       <c r="A36" s="50" t="s">
-        <v>528</v>
+        <v>527</v>
       </c>
       <c r="B36" s="52" t="s">
-        <v>494</v>
+        <v>493</v>
       </c>
       <c r="C36" s="41"/>
       <c r="D36" s="41"/>
       <c r="E36" s="52" t="s">
-        <v>494</v>
+        <v>493</v>
       </c>
       <c r="F36" s="41"/>
       <c r="G36" s="52" t="s">
-        <v>494</v>
+        <v>493</v>
       </c>
       <c r="H36" s="41"/>
       <c r="I36" s="41"/>
@@ -37171,16 +37170,16 @@
     </row>
     <row r="37" ht="15.75" customHeight="1">
       <c r="A37" s="50" t="s">
-        <v>529</v>
+        <v>528</v>
       </c>
       <c r="B37" s="52" t="s">
-        <v>494</v>
+        <v>493</v>
       </c>
       <c r="C37" s="52" t="s">
-        <v>494</v>
+        <v>493</v>
       </c>
       <c r="D37" s="52" t="s">
-        <v>494</v>
+        <v>493</v>
       </c>
       <c r="E37" s="41"/>
       <c r="F37" s="41"/>
@@ -37207,16 +37206,16 @@
     </row>
     <row r="38" ht="15.75" customHeight="1">
       <c r="A38" s="50" t="s">
-        <v>530</v>
+        <v>529</v>
       </c>
       <c r="B38" s="52" t="s">
-        <v>494</v>
+        <v>493</v>
       </c>
       <c r="C38" s="52" t="s">
-        <v>494</v>
+        <v>493</v>
       </c>
       <c r="D38" s="52" t="s">
-        <v>494</v>
+        <v>493</v>
       </c>
       <c r="E38" s="41"/>
       <c r="F38" s="41"/>
@@ -37243,14 +37242,14 @@
     </row>
     <row r="39" ht="15.75" customHeight="1">
       <c r="A39" s="50" t="s">
-        <v>531</v>
+        <v>530</v>
       </c>
       <c r="B39" s="52" t="s">
-        <v>494</v>
+        <v>493</v>
       </c>
       <c r="C39" s="41"/>
       <c r="D39" s="52" t="s">
-        <v>494</v>
+        <v>493</v>
       </c>
       <c r="E39" s="41"/>
       <c r="F39" s="41"/>
@@ -37277,16 +37276,16 @@
     </row>
     <row r="40" ht="15.75" customHeight="1">
       <c r="A40" s="50" t="s">
-        <v>532</v>
+        <v>531</v>
       </c>
       <c r="B40" s="52" t="s">
-        <v>494</v>
+        <v>493</v>
       </c>
       <c r="C40" s="52" t="s">
-        <v>494</v>
+        <v>493</v>
       </c>
       <c r="D40" s="52" t="s">
-        <v>494</v>
+        <v>493</v>
       </c>
       <c r="E40" s="41"/>
       <c r="F40" s="41"/>
@@ -37313,10 +37312,10 @@
     </row>
     <row r="41" ht="15.75" customHeight="1">
       <c r="A41" s="50" t="s">
-        <v>533</v>
+        <v>532</v>
       </c>
       <c r="B41" s="52" t="s">
-        <v>494</v>
+        <v>493</v>
       </c>
       <c r="C41" s="42"/>
       <c r="D41" s="41"/>
@@ -37345,16 +37344,16 @@
     </row>
     <row r="42" ht="15.75" customHeight="1">
       <c r="A42" s="50" t="s">
-        <v>534</v>
+        <v>533</v>
       </c>
       <c r="B42" s="52" t="s">
-        <v>494</v>
+        <v>493</v>
       </c>
       <c r="C42" s="52" t="s">
-        <v>494</v>
+        <v>493</v>
       </c>
       <c r="D42" s="52" t="s">
-        <v>494</v>
+        <v>493</v>
       </c>
       <c r="E42" s="41"/>
       <c r="F42" s="41"/>
@@ -37381,10 +37380,10 @@
     </row>
     <row r="43" ht="15.75" customHeight="1">
       <c r="A43" s="50" t="s">
-        <v>535</v>
+        <v>534</v>
       </c>
       <c r="B43" s="52" t="s">
-        <v>494</v>
+        <v>493</v>
       </c>
       <c r="C43" s="41"/>
       <c r="D43" s="41"/>
@@ -37413,10 +37412,10 @@
     </row>
     <row r="44" ht="15.75" customHeight="1">
       <c r="A44" s="50" t="s">
-        <v>536</v>
+        <v>535</v>
       </c>
       <c r="B44" s="52" t="s">
-        <v>494</v>
+        <v>493</v>
       </c>
       <c r="C44" s="42"/>
       <c r="D44" s="41"/>
@@ -37445,14 +37444,14 @@
     </row>
     <row r="45" ht="15.75" customHeight="1">
       <c r="A45" s="50" t="s">
-        <v>537</v>
+        <v>536</v>
       </c>
       <c r="B45" s="52" t="s">
-        <v>494</v>
+        <v>493</v>
       </c>
       <c r="C45" s="41"/>
       <c r="D45" s="52" t="s">
-        <v>494</v>
+        <v>493</v>
       </c>
       <c r="E45" s="41"/>
       <c r="F45" s="41"/>
@@ -37479,10 +37478,10 @@
     </row>
     <row r="46" ht="15.75" customHeight="1">
       <c r="A46" s="50" t="s">
-        <v>538</v>
+        <v>537</v>
       </c>
       <c r="B46" s="52" t="s">
-        <v>494</v>
+        <v>493</v>
       </c>
       <c r="C46" s="42"/>
       <c r="D46" s="41"/>
@@ -37511,14 +37510,14 @@
     </row>
     <row r="47" ht="15.75" customHeight="1">
       <c r="A47" s="50" t="s">
-        <v>539</v>
+        <v>538</v>
       </c>
       <c r="B47" s="52" t="s">
-        <v>494</v>
+        <v>493</v>
       </c>
       <c r="C47" s="41"/>
       <c r="D47" s="52" t="s">
-        <v>494</v>
+        <v>493</v>
       </c>
       <c r="E47" s="41"/>
       <c r="F47" s="41"/>
@@ -37545,14 +37544,14 @@
     </row>
     <row r="48" ht="15.75" customHeight="1">
       <c r="A48" s="50" t="s">
-        <v>540</v>
+        <v>539</v>
       </c>
       <c r="B48" s="52" t="s">
-        <v>494</v>
+        <v>493</v>
       </c>
       <c r="C48" s="42"/>
       <c r="D48" s="52" t="s">
-        <v>494</v>
+        <v>493</v>
       </c>
       <c r="E48" s="41"/>
       <c r="F48" s="41"/>
@@ -37579,14 +37578,14 @@
     </row>
     <row r="49" ht="15.75" customHeight="1">
       <c r="A49" s="50" t="s">
-        <v>541</v>
+        <v>540</v>
       </c>
       <c r="B49" s="52" t="s">
-        <v>494</v>
+        <v>493</v>
       </c>
       <c r="C49" s="41"/>
       <c r="D49" s="52" t="s">
-        <v>494</v>
+        <v>493</v>
       </c>
       <c r="E49" s="41"/>
       <c r="F49" s="41"/>
@@ -37613,17 +37612,17 @@
     </row>
     <row r="50" ht="15.75" customHeight="1">
       <c r="A50" s="50" t="s">
-        <v>542</v>
+        <v>541</v>
       </c>
       <c r="B50" s="52" t="s">
-        <v>494</v>
+        <v>493</v>
       </c>
       <c r="C50" s="41"/>
       <c r="D50" s="55"/>
       <c r="E50" s="41"/>
       <c r="F50" s="41"/>
       <c r="G50" s="52" t="s">
-        <v>494</v>
+        <v>493</v>
       </c>
       <c r="H50" s="41"/>
       <c r="I50" s="41"/>
@@ -37647,10 +37646,10 @@
     </row>
     <row r="51" ht="15.75" customHeight="1">
       <c r="A51" s="50" t="s">
-        <v>543</v>
+        <v>542</v>
       </c>
       <c r="B51" s="52" t="s">
-        <v>494</v>
+        <v>493</v>
       </c>
       <c r="C51" s="41"/>
       <c r="D51" s="41"/>
@@ -37679,17 +37678,17 @@
     </row>
     <row r="52" ht="15.75" customHeight="1">
       <c r="A52" s="50" t="s">
-        <v>544</v>
+        <v>543</v>
       </c>
       <c r="B52" s="52" t="s">
-        <v>494</v>
+        <v>493</v>
       </c>
       <c r="C52" s="41"/>
       <c r="D52" s="41"/>
       <c r="E52" s="41"/>
       <c r="F52" s="41"/>
       <c r="G52" s="52" t="s">
-        <v>494</v>
+        <v>493</v>
       </c>
       <c r="H52" s="41"/>
       <c r="I52" s="41"/>
@@ -37713,13 +37712,13 @@
     </row>
     <row r="53" ht="15.75" customHeight="1">
       <c r="A53" s="50" t="s">
-        <v>545</v>
+        <v>544</v>
       </c>
       <c r="B53" s="52" t="s">
-        <v>494</v>
+        <v>493</v>
       </c>
       <c r="C53" s="52" t="s">
-        <v>494</v>
+        <v>493</v>
       </c>
       <c r="D53" s="41"/>
       <c r="E53" s="41"/>
@@ -37747,15 +37746,15 @@
     </row>
     <row r="54" ht="15.75" customHeight="1">
       <c r="A54" s="50" t="s">
-        <v>546</v>
+        <v>545</v>
       </c>
       <c r="B54" s="52" t="s">
-        <v>494</v>
+        <v>493</v>
       </c>
       <c r="C54" s="42"/>
       <c r="D54" s="41"/>
       <c r="E54" s="52" t="s">
-        <v>494</v>
+        <v>493</v>
       </c>
       <c r="F54" s="41"/>
       <c r="G54" s="41"/>
@@ -37781,10 +37780,10 @@
     </row>
     <row r="55" ht="15.75" customHeight="1">
       <c r="A55" s="50" t="s">
-        <v>547</v>
+        <v>546</v>
       </c>
       <c r="B55" s="52" t="s">
-        <v>494</v>
+        <v>493</v>
       </c>
       <c r="C55" s="41"/>
       <c r="D55" s="41"/>
@@ -37813,14 +37812,14 @@
     </row>
     <row r="56" ht="15.75" customHeight="1">
       <c r="A56" s="50" t="s">
-        <v>548</v>
+        <v>547</v>
       </c>
       <c r="B56" s="52" t="s">
-        <v>494</v>
+        <v>493</v>
       </c>
       <c r="C56" s="41"/>
       <c r="D56" s="52" t="s">
-        <v>494</v>
+        <v>493</v>
       </c>
       <c r="E56" s="41"/>
       <c r="F56" s="41"/>
@@ -37847,14 +37846,14 @@
     </row>
     <row r="57" ht="15.75" customHeight="1">
       <c r="A57" s="50" t="s">
-        <v>549</v>
+        <v>548</v>
       </c>
       <c r="B57" s="52" t="s">
-        <v>494</v>
+        <v>493</v>
       </c>
       <c r="C57" s="42"/>
       <c r="D57" s="52" t="s">
-        <v>494</v>
+        <v>493</v>
       </c>
       <c r="E57" s="41"/>
       <c r="F57" s="41"/>
@@ -37881,16 +37880,16 @@
     </row>
     <row r="58" ht="15.75" customHeight="1">
       <c r="A58" s="50" t="s">
-        <v>550</v>
+        <v>549</v>
       </c>
       <c r="B58" s="52" t="s">
-        <v>494</v>
+        <v>493</v>
       </c>
       <c r="C58" s="52" t="s">
-        <v>494</v>
+        <v>493</v>
       </c>
       <c r="D58" s="52" t="s">
-        <v>494</v>
+        <v>493</v>
       </c>
       <c r="E58" s="41"/>
       <c r="F58" s="41"/>
@@ -37917,16 +37916,16 @@
     </row>
     <row r="59" ht="15.75" customHeight="1">
       <c r="A59" s="50" t="s">
-        <v>551</v>
+        <v>550</v>
       </c>
       <c r="B59" s="52" t="s">
-        <v>494</v>
+        <v>493</v>
       </c>
       <c r="C59" s="52" t="s">
-        <v>494</v>
+        <v>493</v>
       </c>
       <c r="D59" s="52" t="s">
-        <v>494</v>
+        <v>493</v>
       </c>
       <c r="E59" s="41"/>
       <c r="F59" s="41"/>
@@ -37953,16 +37952,16 @@
     </row>
     <row r="60" ht="15.75" customHeight="1">
       <c r="A60" s="50" t="s">
-        <v>552</v>
+        <v>551</v>
       </c>
       <c r="B60" s="52" t="s">
-        <v>494</v>
+        <v>493</v>
       </c>
       <c r="C60" s="52" t="s">
-        <v>494</v>
+        <v>493</v>
       </c>
       <c r="D60" s="52" t="s">
-        <v>494</v>
+        <v>493</v>
       </c>
       <c r="E60" s="41"/>
       <c r="F60" s="41"/>
@@ -37989,16 +37988,16 @@
     </row>
     <row r="61" ht="15.75" customHeight="1">
       <c r="A61" s="50" t="s">
-        <v>553</v>
+        <v>552</v>
       </c>
       <c r="B61" s="52" t="s">
-        <v>494</v>
+        <v>493</v>
       </c>
       <c r="C61" s="52" t="s">
-        <v>494</v>
+        <v>493</v>
       </c>
       <c r="D61" s="52" t="s">
-        <v>494</v>
+        <v>493</v>
       </c>
       <c r="E61" s="41"/>
       <c r="F61" s="41"/>
@@ -38025,18 +38024,18 @@
     </row>
     <row r="62" ht="15.75" customHeight="1">
       <c r="A62" s="50" t="s">
-        <v>554</v>
+        <v>553</v>
       </c>
       <c r="B62" s="52" t="s">
-        <v>494</v>
+        <v>493</v>
       </c>
       <c r="C62" s="52"/>
       <c r="D62" s="52" t="s">
-        <v>494</v>
+        <v>493</v>
       </c>
       <c r="E62" s="41"/>
       <c r="F62" s="52" t="s">
-        <v>494</v>
+        <v>493</v>
       </c>
       <c r="G62" s="56"/>
       <c r="H62" s="41"/>
@@ -38061,16 +38060,16 @@
     </row>
     <row r="63" ht="15.75" customHeight="1">
       <c r="A63" s="50" t="s">
-        <v>555</v>
+        <v>554</v>
       </c>
       <c r="B63" s="52" t="s">
-        <v>494</v>
+        <v>493</v>
       </c>
       <c r="C63" s="52" t="s">
-        <v>494</v>
+        <v>493</v>
       </c>
       <c r="D63" s="52" t="s">
-        <v>494</v>
+        <v>493</v>
       </c>
       <c r="E63" s="41"/>
       <c r="F63" s="41"/>
@@ -38097,25 +38096,25 @@
     </row>
     <row r="64" ht="15.75" customHeight="1">
       <c r="A64" s="50" t="s">
-        <v>556</v>
+        <v>555</v>
       </c>
       <c r="B64" s="52" t="s">
-        <v>494</v>
+        <v>493</v>
       </c>
       <c r="C64" s="52" t="s">
-        <v>494</v>
+        <v>493</v>
       </c>
       <c r="D64" s="52" t="s">
-        <v>494</v>
+        <v>493</v>
       </c>
       <c r="E64" s="52" t="s">
-        <v>494</v>
+        <v>493</v>
       </c>
       <c r="F64" s="52" t="s">
-        <v>494</v>
+        <v>493</v>
       </c>
       <c r="G64" s="52" t="s">
-        <v>494</v>
+        <v>493</v>
       </c>
       <c r="H64" s="41"/>
       <c r="I64" s="41"/>
@@ -38139,14 +38138,14 @@
     </row>
     <row r="65" ht="15.75" customHeight="1">
       <c r="A65" s="50" t="s">
-        <v>557</v>
+        <v>556</v>
       </c>
       <c r="B65" s="52" t="s">
-        <v>494</v>
+        <v>493</v>
       </c>
       <c r="C65" s="41"/>
       <c r="D65" s="52" t="s">
-        <v>494</v>
+        <v>493</v>
       </c>
       <c r="E65" s="41"/>
       <c r="F65" s="41"/>
@@ -38173,16 +38172,16 @@
     </row>
     <row r="66" ht="15.75" customHeight="1">
       <c r="A66" s="50" t="s">
-        <v>558</v>
+        <v>557</v>
       </c>
       <c r="B66" s="52" t="s">
-        <v>494</v>
+        <v>493</v>
       </c>
       <c r="C66" s="52" t="s">
-        <v>494</v>
+        <v>493</v>
       </c>
       <c r="D66" s="52" t="s">
-        <v>494</v>
+        <v>493</v>
       </c>
       <c r="E66" s="41"/>
       <c r="F66" s="41"/>
@@ -38209,10 +38208,10 @@
     </row>
     <row r="67" ht="15.75" customHeight="1">
       <c r="A67" s="50" t="s">
-        <v>559</v>
+        <v>558</v>
       </c>
       <c r="B67" s="52" t="s">
-        <v>494</v>
+        <v>493</v>
       </c>
       <c r="C67" s="42"/>
       <c r="D67" s="41"/>
@@ -38241,14 +38240,14 @@
     </row>
     <row r="68" ht="15.75" customHeight="1">
       <c r="A68" s="50" t="s">
-        <v>560</v>
+        <v>559</v>
       </c>
       <c r="B68" s="52" t="s">
-        <v>494</v>
+        <v>493</v>
       </c>
       <c r="C68" s="41"/>
       <c r="D68" s="52" t="s">
-        <v>494</v>
+        <v>493</v>
       </c>
       <c r="E68" s="41"/>
       <c r="F68" s="41"/>
@@ -38275,13 +38274,13 @@
     </row>
     <row r="69" ht="15.75" customHeight="1">
       <c r="A69" s="50" t="s">
-        <v>561</v>
+        <v>560</v>
       </c>
       <c r="B69" s="52" t="s">
-        <v>494</v>
+        <v>493</v>
       </c>
       <c r="C69" s="52" t="s">
-        <v>494</v>
+        <v>493</v>
       </c>
       <c r="D69" s="41"/>
       <c r="E69" s="41"/>
@@ -38309,10 +38308,10 @@
     </row>
     <row r="70" ht="15.75" customHeight="1">
       <c r="A70" s="50" t="s">
-        <v>562</v>
+        <v>561</v>
       </c>
       <c r="B70" s="52" t="s">
-        <v>494</v>
+        <v>493</v>
       </c>
       <c r="C70" s="41"/>
       <c r="D70" s="41"/>
@@ -38341,17 +38340,17 @@
     </row>
     <row r="71" ht="15.75" customHeight="1">
       <c r="A71" s="50" t="s">
-        <v>563</v>
+        <v>562</v>
       </c>
       <c r="B71" s="52" t="s">
-        <v>494</v>
+        <v>493</v>
       </c>
       <c r="C71" s="52" t="s">
-        <v>494</v>
+        <v>493</v>
       </c>
       <c r="D71" s="41"/>
       <c r="E71" s="52" t="s">
-        <v>494</v>
+        <v>493</v>
       </c>
       <c r="F71" s="41"/>
       <c r="G71" s="41"/>
@@ -38377,14 +38376,14 @@
     </row>
     <row r="72" ht="15.75" customHeight="1">
       <c r="A72" s="50" t="s">
-        <v>564</v>
+        <v>563</v>
       </c>
       <c r="B72" s="52" t="s">
-        <v>494</v>
+        <v>493</v>
       </c>
       <c r="C72" s="42"/>
       <c r="D72" s="52" t="s">
-        <v>494</v>
+        <v>493</v>
       </c>
       <c r="E72" s="41"/>
       <c r="F72" s="41"/>
@@ -38411,14 +38410,14 @@
     </row>
     <row r="73" ht="15.75" customHeight="1">
       <c r="A73" s="50" t="s">
-        <v>565</v>
+        <v>564</v>
       </c>
       <c r="B73" s="52" t="s">
-        <v>494</v>
+        <v>493</v>
       </c>
       <c r="C73" s="42"/>
       <c r="D73" s="52" t="s">
-        <v>494</v>
+        <v>493</v>
       </c>
       <c r="E73" s="41"/>
       <c r="F73" s="41"/>
@@ -38445,14 +38444,14 @@
     </row>
     <row r="74" ht="15.75" customHeight="1">
       <c r="A74" s="50" t="s">
-        <v>566</v>
+        <v>565</v>
       </c>
       <c r="B74" s="52" t="s">
-        <v>494</v>
+        <v>493</v>
       </c>
       <c r="C74" s="41"/>
       <c r="D74" s="52" t="s">
-        <v>494</v>
+        <v>493</v>
       </c>
       <c r="E74" s="41"/>
       <c r="F74" s="41"/>
@@ -38479,14 +38478,14 @@
     </row>
     <row r="75" ht="15.75" customHeight="1">
       <c r="A75" s="50" t="s">
-        <v>567</v>
+        <v>566</v>
       </c>
       <c r="B75" s="52" t="s">
-        <v>494</v>
+        <v>493</v>
       </c>
       <c r="C75" s="41"/>
       <c r="D75" s="52" t="s">
-        <v>494</v>
+        <v>493</v>
       </c>
       <c r="E75" s="41"/>
       <c r="F75" s="41"/>
@@ -38513,14 +38512,14 @@
     </row>
     <row r="76" ht="15.75" customHeight="1">
       <c r="A76" s="50" t="s">
-        <v>568</v>
+        <v>567</v>
       </c>
       <c r="B76" s="52" t="s">
-        <v>494</v>
+        <v>493</v>
       </c>
       <c r="C76" s="41"/>
       <c r="D76" s="52" t="s">
-        <v>494</v>
+        <v>493</v>
       </c>
       <c r="E76" s="41"/>
       <c r="F76" s="41"/>
@@ -38547,17 +38546,17 @@
     </row>
     <row r="77" ht="15.75" customHeight="1">
       <c r="A77" s="50" t="s">
-        <v>569</v>
+        <v>568</v>
       </c>
       <c r="B77" s="52" t="s">
-        <v>494</v>
+        <v>493</v>
       </c>
       <c r="C77" s="42"/>
       <c r="D77" s="42"/>
       <c r="E77" s="41"/>
       <c r="F77" s="41"/>
       <c r="G77" s="52" t="s">
-        <v>494</v>
+        <v>493</v>
       </c>
       <c r="H77" s="41"/>
       <c r="I77" s="41"/>
@@ -38581,10 +38580,10 @@
     </row>
     <row r="78" ht="15.75" customHeight="1">
       <c r="A78" s="50" t="s">
-        <v>570</v>
+        <v>569</v>
       </c>
       <c r="B78" s="52" t="s">
-        <v>494</v>
+        <v>493</v>
       </c>
       <c r="C78" s="42"/>
       <c r="D78" s="41"/>
@@ -38613,16 +38612,16 @@
     </row>
     <row r="79" ht="15.75" customHeight="1">
       <c r="A79" s="50" t="s">
-        <v>571</v>
+        <v>570</v>
       </c>
       <c r="B79" s="52" t="s">
-        <v>494</v>
+        <v>493</v>
       </c>
       <c r="C79" s="52" t="s">
-        <v>494</v>
+        <v>493</v>
       </c>
       <c r="D79" s="52" t="s">
-        <v>494</v>
+        <v>493</v>
       </c>
       <c r="E79" s="41"/>
       <c r="F79" s="41"/>
@@ -38649,13 +38648,13 @@
     </row>
     <row r="80" ht="15.75" customHeight="1">
       <c r="A80" s="50" t="s">
-        <v>572</v>
+        <v>571</v>
       </c>
       <c r="B80" s="52" t="s">
-        <v>494</v>
+        <v>493</v>
       </c>
       <c r="C80" s="52" t="s">
-        <v>494</v>
+        <v>493</v>
       </c>
       <c r="D80" s="41"/>
       <c r="E80" s="41"/>
@@ -38683,19 +38682,19 @@
     </row>
     <row r="81" ht="15.75" customHeight="1">
       <c r="A81" s="50" t="s">
-        <v>573</v>
+        <v>572</v>
       </c>
       <c r="B81" s="52" t="s">
-        <v>494</v>
+        <v>493</v>
       </c>
       <c r="C81" s="52" t="s">
-        <v>494</v>
+        <v>493</v>
       </c>
       <c r="D81" s="52" t="s">
-        <v>494</v>
+        <v>493</v>
       </c>
       <c r="E81" s="52" t="s">
-        <v>494</v>
+        <v>493</v>
       </c>
       <c r="F81" s="41"/>
       <c r="G81" s="41"/>
@@ -38721,19 +38720,19 @@
     </row>
     <row r="82" ht="15.75" customHeight="1">
       <c r="A82" s="50" t="s">
-        <v>574</v>
+        <v>573</v>
       </c>
       <c r="B82" s="52" t="s">
-        <v>494</v>
+        <v>493</v>
       </c>
       <c r="C82" s="52" t="s">
-        <v>494</v>
+        <v>493</v>
       </c>
       <c r="D82" s="56"/>
       <c r="E82" s="41"/>
       <c r="F82" s="41"/>
       <c r="G82" s="52" t="s">
-        <v>494</v>
+        <v>493</v>
       </c>
       <c r="H82" s="41"/>
       <c r="I82" s="41"/>
@@ -38757,17 +38756,17 @@
     </row>
     <row r="83" ht="15.75" customHeight="1">
       <c r="A83" s="50" t="s">
-        <v>575</v>
+        <v>574</v>
       </c>
       <c r="B83" s="52" t="s">
-        <v>494</v>
+        <v>493</v>
       </c>
       <c r="C83" s="41"/>
       <c r="D83" s="41"/>
       <c r="E83" s="41"/>
       <c r="F83" s="41"/>
       <c r="G83" s="52" t="s">
-        <v>494</v>
+        <v>493</v>
       </c>
       <c r="H83" s="41"/>
       <c r="I83" s="41"/>
@@ -38791,17 +38790,17 @@
     </row>
     <row r="84" ht="15.75" customHeight="1">
       <c r="A84" s="50" t="s">
-        <v>576</v>
+        <v>575</v>
       </c>
       <c r="B84" s="52" t="s">
-        <v>494</v>
+        <v>493</v>
       </c>
       <c r="C84" s="41"/>
       <c r="D84" s="41"/>
       <c r="E84" s="41"/>
       <c r="F84" s="41"/>
       <c r="G84" s="52" t="s">
-        <v>494</v>
+        <v>493</v>
       </c>
       <c r="H84" s="41"/>
       <c r="I84" s="41"/>
@@ -38825,17 +38824,17 @@
     </row>
     <row r="85" ht="15.75" customHeight="1">
       <c r="A85" s="50" t="s">
-        <v>577</v>
+        <v>576</v>
       </c>
       <c r="B85" s="52" t="s">
-        <v>494</v>
+        <v>493</v>
       </c>
       <c r="C85" s="41"/>
       <c r="D85" s="41"/>
       <c r="E85" s="41"/>
       <c r="F85" s="41"/>
       <c r="G85" s="52" t="s">
-        <v>494</v>
+        <v>493</v>
       </c>
       <c r="H85" s="41"/>
       <c r="I85" s="41"/>
@@ -38859,16 +38858,16 @@
     </row>
     <row r="86" ht="15.75" customHeight="1">
       <c r="A86" s="50" t="s">
-        <v>578</v>
+        <v>577</v>
       </c>
       <c r="B86" s="52" t="s">
-        <v>494</v>
+        <v>493</v>
       </c>
       <c r="C86" s="52" t="s">
-        <v>494</v>
+        <v>493</v>
       </c>
       <c r="D86" s="52" t="s">
-        <v>494</v>
+        <v>493</v>
       </c>
       <c r="E86" s="41"/>
       <c r="F86" s="41"/>
@@ -38895,10 +38894,10 @@
     </row>
     <row r="87" ht="15.75" customHeight="1">
       <c r="A87" s="50" t="s">
-        <v>579</v>
+        <v>578</v>
       </c>
       <c r="B87" s="52" t="s">
-        <v>494</v>
+        <v>493</v>
       </c>
       <c r="C87" s="41"/>
       <c r="D87" s="41"/>
@@ -38927,13 +38926,13 @@
     </row>
     <row r="88" ht="15.75" customHeight="1">
       <c r="A88" s="50" t="s">
-        <v>580</v>
+        <v>579</v>
       </c>
       <c r="B88" s="52" t="s">
-        <v>494</v>
+        <v>493</v>
       </c>
       <c r="C88" s="52" t="s">
-        <v>494</v>
+        <v>493</v>
       </c>
       <c r="D88" s="41"/>
       <c r="E88" s="41"/>
@@ -38961,21 +38960,21 @@
     </row>
     <row r="89" ht="15.75" customHeight="1">
       <c r="A89" s="50" t="s">
-        <v>581</v>
+        <v>580</v>
       </c>
       <c r="B89" s="52" t="s">
-        <v>494</v>
+        <v>493</v>
       </c>
       <c r="C89" s="52" t="s">
-        <v>494</v>
+        <v>493</v>
       </c>
       <c r="D89" s="41"/>
       <c r="E89" s="52" t="s">
-        <v>494</v>
+        <v>493</v>
       </c>
       <c r="F89" s="41"/>
       <c r="G89" s="52" t="s">
-        <v>494</v>
+        <v>493</v>
       </c>
       <c r="H89" s="41"/>
       <c r="I89" s="41"/>
@@ -38999,10 +38998,10 @@
     </row>
     <row r="90" ht="15.75" customHeight="1">
       <c r="A90" s="50" t="s">
-        <v>582</v>
+        <v>581</v>
       </c>
       <c r="B90" s="52" t="s">
-        <v>494</v>
+        <v>493</v>
       </c>
       <c r="C90" s="41"/>
       <c r="D90" s="41"/>
@@ -39031,10 +39030,10 @@
     </row>
     <row r="91" ht="15.75" customHeight="1">
       <c r="A91" s="50" t="s">
-        <v>583</v>
+        <v>582</v>
       </c>
       <c r="B91" s="52" t="s">
-        <v>494</v>
+        <v>493</v>
       </c>
       <c r="C91" s="42"/>
       <c r="D91" s="42"/>
@@ -39063,10 +39062,10 @@
     </row>
     <row r="92" ht="15.75" customHeight="1">
       <c r="A92" s="50" t="s">
-        <v>584</v>
+        <v>583</v>
       </c>
       <c r="B92" s="52" t="s">
-        <v>494</v>
+        <v>493</v>
       </c>
       <c r="C92" s="42"/>
       <c r="D92" s="41"/>
@@ -39095,10 +39094,10 @@
     </row>
     <row r="93" ht="15.75" customHeight="1">
       <c r="A93" s="50" t="s">
-        <v>585</v>
+        <v>584</v>
       </c>
       <c r="B93" s="52" t="s">
-        <v>494</v>
+        <v>493</v>
       </c>
       <c r="C93" s="41"/>
       <c r="D93" s="42"/>
@@ -39127,14 +39126,14 @@
     </row>
     <row r="94" ht="15.75" customHeight="1">
       <c r="A94" s="50" t="s">
-        <v>586</v>
+        <v>585</v>
       </c>
       <c r="B94" s="52" t="s">
-        <v>494</v>
+        <v>493</v>
       </c>
       <c r="C94" s="42"/>
       <c r="D94" s="52" t="s">
-        <v>494</v>
+        <v>493</v>
       </c>
       <c r="E94" s="41"/>
       <c r="F94" s="41"/>
@@ -39161,21 +39160,21 @@
     </row>
     <row r="95" ht="15.75" customHeight="1">
       <c r="A95" s="50" t="s">
-        <v>587</v>
+        <v>586</v>
       </c>
       <c r="B95" s="52" t="s">
-        <v>494</v>
+        <v>493</v>
       </c>
       <c r="C95" s="42"/>
       <c r="D95" s="52" t="s">
-        <v>494</v>
+        <v>493</v>
       </c>
       <c r="E95" s="52" t="s">
-        <v>494</v>
+        <v>493</v>
       </c>
       <c r="F95" s="41"/>
       <c r="G95" s="52" t="s">
-        <v>494</v>
+        <v>493</v>
       </c>
       <c r="H95" s="41"/>
       <c r="I95" s="41"/>
@@ -39199,13 +39198,13 @@
     </row>
     <row r="96" ht="15.75" customHeight="1">
       <c r="A96" s="50" t="s">
-        <v>588</v>
+        <v>587</v>
       </c>
       <c r="B96" s="52" t="s">
-        <v>494</v>
+        <v>493</v>
       </c>
       <c r="C96" s="52" t="s">
-        <v>494</v>
+        <v>493</v>
       </c>
       <c r="D96" s="41"/>
       <c r="E96" s="41"/>
@@ -39233,13 +39232,13 @@
     </row>
     <row r="97" ht="15.75" customHeight="1">
       <c r="A97" s="50" t="s">
-        <v>589</v>
+        <v>588</v>
       </c>
       <c r="B97" s="52" t="s">
-        <v>494</v>
+        <v>493</v>
       </c>
       <c r="C97" s="52" t="s">
-        <v>494</v>
+        <v>493</v>
       </c>
       <c r="D97" s="41"/>
       <c r="E97" s="41"/>
@@ -39267,13 +39266,13 @@
     </row>
     <row r="98" ht="15.75" customHeight="1">
       <c r="A98" s="50" t="s">
-        <v>590</v>
+        <v>589</v>
       </c>
       <c r="B98" s="52" t="s">
-        <v>494</v>
+        <v>493</v>
       </c>
       <c r="C98" s="52" t="s">
-        <v>494</v>
+        <v>493</v>
       </c>
       <c r="D98" s="41"/>
       <c r="E98" s="41"/>
@@ -39301,11 +39300,11 @@
     </row>
     <row r="99" ht="15.75" customHeight="1">
       <c r="A99" s="50" t="s">
-        <v>591</v>
+        <v>590</v>
       </c>
       <c r="B99" s="56"/>
       <c r="C99" s="52" t="s">
-        <v>494</v>
+        <v>493</v>
       </c>
       <c r="D99" s="41"/>
       <c r="E99" s="41"/>
@@ -39333,16 +39332,16 @@
     </row>
     <row r="100" ht="15.75" customHeight="1">
       <c r="A100" s="50" t="s">
-        <v>592</v>
+        <v>591</v>
       </c>
       <c r="B100" s="52" t="s">
-        <v>494</v>
+        <v>493</v>
       </c>
       <c r="C100" s="52" t="s">
-        <v>494</v>
+        <v>493</v>
       </c>
       <c r="D100" s="52" t="s">
-        <v>494</v>
+        <v>493</v>
       </c>
       <c r="E100" s="41"/>
       <c r="F100" s="41"/>
@@ -39369,16 +39368,16 @@
     </row>
     <row r="101" ht="15.75" customHeight="1">
       <c r="A101" s="50" t="s">
-        <v>593</v>
+        <v>592</v>
       </c>
       <c r="B101" s="52" t="s">
-        <v>494</v>
+        <v>493</v>
       </c>
       <c r="C101" s="52" t="s">
-        <v>494</v>
+        <v>493</v>
       </c>
       <c r="D101" s="52" t="s">
-        <v>494</v>
+        <v>493</v>
       </c>
       <c r="E101" s="41"/>
       <c r="F101" s="41"/>
@@ -39405,16 +39404,16 @@
     </row>
     <row r="102" ht="15.75" customHeight="1">
       <c r="A102" s="50" t="s">
-        <v>594</v>
+        <v>593</v>
       </c>
       <c r="B102" s="52" t="s">
-        <v>494</v>
+        <v>493</v>
       </c>
       <c r="C102" s="52" t="s">
-        <v>494</v>
+        <v>493</v>
       </c>
       <c r="D102" s="52" t="s">
-        <v>494</v>
+        <v>493</v>
       </c>
       <c r="E102" s="41"/>
       <c r="F102" s="41"/>
@@ -39441,16 +39440,16 @@
     </row>
     <row r="103" ht="15.75" customHeight="1">
       <c r="A103" s="50" t="s">
-        <v>595</v>
+        <v>594</v>
       </c>
       <c r="B103" s="52" t="s">
-        <v>494</v>
+        <v>493</v>
       </c>
       <c r="C103" s="52" t="s">
-        <v>494</v>
+        <v>493</v>
       </c>
       <c r="D103" s="52" t="s">
-        <v>494</v>
+        <v>493</v>
       </c>
       <c r="E103" s="41"/>
       <c r="F103" s="41"/>
@@ -39477,16 +39476,16 @@
     </row>
     <row r="104" ht="15.75" customHeight="1">
       <c r="A104" s="50" t="s">
-        <v>596</v>
+        <v>595</v>
       </c>
       <c r="B104" s="52" t="s">
-        <v>494</v>
+        <v>493</v>
       </c>
       <c r="C104" s="52" t="s">
-        <v>494</v>
+        <v>493</v>
       </c>
       <c r="D104" s="52" t="s">
-        <v>494</v>
+        <v>493</v>
       </c>
       <c r="E104" s="41"/>
       <c r="F104" s="41"/>
@@ -39513,14 +39512,14 @@
     </row>
     <row r="105" ht="15.75" customHeight="1">
       <c r="A105" s="50" t="s">
-        <v>597</v>
+        <v>596</v>
       </c>
       <c r="B105" s="52" t="s">
-        <v>494</v>
+        <v>493</v>
       </c>
       <c r="C105" s="41"/>
       <c r="D105" s="52" t="s">
-        <v>494</v>
+        <v>493</v>
       </c>
       <c r="E105" s="41"/>
       <c r="F105" s="41"/>
@@ -39547,14 +39546,14 @@
     </row>
     <row r="106" ht="15.75" customHeight="1">
       <c r="A106" s="50" t="s">
-        <v>598</v>
+        <v>597</v>
       </c>
       <c r="B106" s="52" t="s">
-        <v>494</v>
+        <v>493</v>
       </c>
       <c r="C106" s="41"/>
       <c r="D106" s="52" t="s">
-        <v>494</v>
+        <v>493</v>
       </c>
       <c r="E106" s="41"/>
       <c r="F106" s="41"/>
@@ -39581,14 +39580,14 @@
     </row>
     <row r="107" ht="15.75" customHeight="1">
       <c r="A107" s="50" t="s">
-        <v>599</v>
+        <v>598</v>
       </c>
       <c r="B107" s="52" t="s">
-        <v>494</v>
+        <v>493</v>
       </c>
       <c r="C107" s="41"/>
       <c r="D107" s="52" t="s">
-        <v>494</v>
+        <v>493</v>
       </c>
       <c r="E107" s="41"/>
       <c r="F107" s="41"/>
@@ -39615,14 +39614,14 @@
     </row>
     <row r="108" ht="15.75" customHeight="1">
       <c r="A108" s="50" t="s">
-        <v>600</v>
+        <v>599</v>
       </c>
       <c r="B108" s="52" t="s">
-        <v>494</v>
+        <v>493</v>
       </c>
       <c r="C108" s="41"/>
       <c r="D108" s="52" t="s">
-        <v>494</v>
+        <v>493</v>
       </c>
       <c r="E108" s="41"/>
       <c r="F108" s="41"/>
@@ -39649,14 +39648,14 @@
     </row>
     <row r="109" ht="15.75" customHeight="1">
       <c r="A109" s="50" t="s">
-        <v>601</v>
+        <v>600</v>
       </c>
       <c r="B109" s="52" t="s">
-        <v>494</v>
+        <v>493</v>
       </c>
       <c r="C109" s="41"/>
       <c r="D109" s="52" t="s">
-        <v>494</v>
+        <v>493</v>
       </c>
       <c r="E109" s="41"/>
       <c r="F109" s="41"/>
@@ -39683,14 +39682,14 @@
     </row>
     <row r="110" ht="15.75" customHeight="1">
       <c r="A110" s="50" t="s">
-        <v>602</v>
+        <v>601</v>
       </c>
       <c r="B110" s="52" t="s">
-        <v>494</v>
+        <v>493</v>
       </c>
       <c r="C110" s="41"/>
       <c r="D110" s="52" t="s">
-        <v>494</v>
+        <v>493</v>
       </c>
       <c r="E110" s="41"/>
       <c r="F110" s="41"/>
@@ -39717,16 +39716,16 @@
     </row>
     <row r="111" ht="15.75" customHeight="1">
       <c r="A111" s="50" t="s">
-        <v>603</v>
+        <v>602</v>
       </c>
       <c r="B111" s="52" t="s">
-        <v>494</v>
+        <v>493</v>
       </c>
       <c r="C111" s="52" t="s">
-        <v>494</v>
+        <v>493</v>
       </c>
       <c r="D111" s="52" t="s">
-        <v>494</v>
+        <v>493</v>
       </c>
       <c r="E111" s="41"/>
       <c r="F111" s="41"/>
@@ -39753,16 +39752,16 @@
     </row>
     <row r="112" ht="15.75" customHeight="1">
       <c r="A112" s="50" t="s">
-        <v>604</v>
+        <v>603</v>
       </c>
       <c r="B112" s="52" t="s">
-        <v>494</v>
+        <v>493</v>
       </c>
       <c r="C112" s="52" t="s">
-        <v>494</v>
+        <v>493</v>
       </c>
       <c r="D112" s="52" t="s">
-        <v>494</v>
+        <v>493</v>
       </c>
       <c r="E112" s="41"/>
       <c r="F112" s="41"/>
@@ -39789,14 +39788,14 @@
     </row>
     <row r="113" ht="15.75" customHeight="1">
       <c r="A113" s="50" t="s">
-        <v>605</v>
+        <v>604</v>
       </c>
       <c r="B113" s="52" t="s">
-        <v>494</v>
+        <v>493</v>
       </c>
       <c r="C113" s="42"/>
       <c r="D113" s="52" t="s">
-        <v>494</v>
+        <v>493</v>
       </c>
       <c r="E113" s="41"/>
       <c r="F113" s="41"/>
@@ -39823,16 +39822,16 @@
     </row>
     <row r="114" ht="15.75" customHeight="1">
       <c r="A114" s="50" t="s">
-        <v>606</v>
+        <v>605</v>
       </c>
       <c r="B114" s="52" t="s">
-        <v>494</v>
+        <v>493</v>
       </c>
       <c r="C114" s="52" t="s">
-        <v>494</v>
+        <v>493</v>
       </c>
       <c r="D114" s="52" t="s">
-        <v>494</v>
+        <v>493</v>
       </c>
       <c r="E114" s="41"/>
       <c r="F114" s="41"/>
@@ -39859,14 +39858,14 @@
     </row>
     <row r="115" ht="15.75" customHeight="1">
       <c r="A115" s="50" t="s">
-        <v>607</v>
+        <v>606</v>
       </c>
       <c r="B115" s="52" t="s">
-        <v>494</v>
+        <v>493</v>
       </c>
       <c r="C115" s="41"/>
       <c r="D115" s="52" t="s">
-        <v>494</v>
+        <v>493</v>
       </c>
       <c r="E115" s="41"/>
       <c r="F115" s="41"/>
@@ -39893,21 +39892,21 @@
     </row>
     <row r="116" ht="15.75" customHeight="1">
       <c r="A116" s="50" t="s">
-        <v>608</v>
+        <v>607</v>
       </c>
       <c r="B116" s="52" t="s">
-        <v>494</v>
+        <v>493</v>
       </c>
       <c r="C116" s="52" t="s">
-        <v>494</v>
+        <v>493</v>
       </c>
       <c r="D116" s="52" t="s">
-        <v>494</v>
+        <v>493</v>
       </c>
       <c r="E116" s="41"/>
       <c r="F116" s="41"/>
       <c r="G116" s="52" t="s">
-        <v>494</v>
+        <v>493</v>
       </c>
       <c r="H116" s="41"/>
       <c r="I116" s="41"/>
@@ -39931,21 +39930,21 @@
     </row>
     <row r="117" ht="15.75" customHeight="1">
       <c r="A117" s="50" t="s">
-        <v>609</v>
+        <v>608</v>
       </c>
       <c r="B117" s="52" t="s">
-        <v>494</v>
+        <v>493</v>
       </c>
       <c r="C117" s="52" t="s">
-        <v>494</v>
+        <v>493</v>
       </c>
       <c r="D117" s="52" t="s">
-        <v>494</v>
+        <v>493</v>
       </c>
       <c r="E117" s="41"/>
       <c r="F117" s="41"/>
       <c r="G117" s="52" t="s">
-        <v>494</v>
+        <v>493</v>
       </c>
       <c r="H117" s="41"/>
       <c r="I117" s="41"/>
@@ -39969,21 +39968,21 @@
     </row>
     <row r="118" ht="15.75" customHeight="1">
       <c r="A118" s="50" t="s">
-        <v>610</v>
+        <v>609</v>
       </c>
       <c r="B118" s="52" t="s">
-        <v>494</v>
+        <v>493</v>
       </c>
       <c r="C118" s="52" t="s">
-        <v>494</v>
+        <v>493</v>
       </c>
       <c r="D118" s="52" t="s">
-        <v>494</v>
+        <v>493</v>
       </c>
       <c r="E118" s="41"/>
       <c r="F118" s="41"/>
       <c r="G118" s="52" t="s">
-        <v>494</v>
+        <v>493</v>
       </c>
       <c r="H118" s="41"/>
       <c r="I118" s="41"/>
@@ -40007,10 +40006,10 @@
     </row>
     <row r="119" ht="15.75" customHeight="1">
       <c r="A119" s="50" t="s">
-        <v>611</v>
+        <v>610</v>
       </c>
       <c r="B119" s="52" t="s">
-        <v>494</v>
+        <v>493</v>
       </c>
       <c r="C119" s="41"/>
       <c r="D119" s="41"/>
@@ -40039,16 +40038,16 @@
     </row>
     <row r="120" ht="15.75" customHeight="1">
       <c r="A120" s="50" t="s">
-        <v>612</v>
+        <v>611</v>
       </c>
       <c r="B120" s="52" t="s">
-        <v>494</v>
+        <v>493</v>
       </c>
       <c r="C120" s="52" t="s">
-        <v>494</v>
+        <v>493</v>
       </c>
       <c r="D120" s="52" t="s">
-        <v>494</v>
+        <v>493</v>
       </c>
       <c r="E120" s="41"/>
       <c r="F120" s="41"/>
@@ -40075,16 +40074,16 @@
     </row>
     <row r="121" ht="15.75" customHeight="1">
       <c r="A121" s="50" t="s">
-        <v>613</v>
+        <v>612</v>
       </c>
       <c r="B121" s="52" t="s">
-        <v>494</v>
+        <v>493</v>
       </c>
       <c r="C121" s="52" t="s">
-        <v>494</v>
+        <v>493</v>
       </c>
       <c r="D121" s="52" t="s">
-        <v>494</v>
+        <v>493</v>
       </c>
       <c r="E121" s="41"/>
       <c r="F121" s="41"/>
@@ -40111,16 +40110,16 @@
     </row>
     <row r="122" ht="15.75" customHeight="1">
       <c r="A122" s="50" t="s">
-        <v>614</v>
+        <v>613</v>
       </c>
       <c r="B122" s="52" t="s">
-        <v>494</v>
+        <v>493</v>
       </c>
       <c r="C122" s="52" t="s">
-        <v>494</v>
+        <v>493</v>
       </c>
       <c r="D122" s="52" t="s">
-        <v>494</v>
+        <v>493</v>
       </c>
       <c r="E122" s="41"/>
       <c r="F122" s="41"/>
@@ -40147,10 +40146,10 @@
     </row>
     <row r="123" ht="15.75" customHeight="1">
       <c r="A123" s="50" t="s">
-        <v>615</v>
+        <v>614</v>
       </c>
       <c r="B123" s="52" t="s">
-        <v>494</v>
+        <v>493</v>
       </c>
       <c r="C123" s="52"/>
       <c r="D123" s="41"/>
@@ -40179,23 +40178,23 @@
     </row>
     <row r="124" ht="15.75" customHeight="1">
       <c r="A124" s="50" t="s">
-        <v>616</v>
+        <v>615</v>
       </c>
       <c r="B124" s="52" t="s">
-        <v>494</v>
+        <v>493</v>
       </c>
       <c r="C124" s="52" t="s">
-        <v>494</v>
+        <v>493</v>
       </c>
       <c r="D124" s="52" t="s">
-        <v>494</v>
+        <v>493</v>
       </c>
       <c r="E124" s="41"/>
       <c r="F124" s="52" t="s">
-        <v>494</v>
+        <v>493</v>
       </c>
       <c r="G124" s="52" t="s">
-        <v>494</v>
+        <v>493</v>
       </c>
       <c r="H124" s="41"/>
       <c r="I124" s="41"/>
@@ -40219,16 +40218,16 @@
     </row>
     <row r="125" ht="15.75" customHeight="1">
       <c r="A125" s="50" t="s">
-        <v>617</v>
+        <v>616</v>
       </c>
       <c r="B125" s="52" t="s">
-        <v>494</v>
+        <v>493</v>
       </c>
       <c r="C125" s="52" t="s">
-        <v>494</v>
+        <v>493</v>
       </c>
       <c r="D125" s="52" t="s">
-        <v>494</v>
+        <v>493</v>
       </c>
       <c r="E125" s="41"/>
       <c r="F125" s="41"/>
@@ -40255,13 +40254,13 @@
     </row>
     <row r="126" ht="15.75" customHeight="1">
       <c r="A126" s="50" t="s">
-        <v>618</v>
+        <v>617</v>
       </c>
       <c r="B126" s="52" t="s">
-        <v>494</v>
+        <v>493</v>
       </c>
       <c r="C126" s="52" t="s">
-        <v>494</v>
+        <v>493</v>
       </c>
       <c r="D126" s="41"/>
       <c r="E126" s="41"/>
@@ -40289,10 +40288,10 @@
     </row>
     <row r="127" ht="15.75" customHeight="1">
       <c r="A127" s="50" t="s">
-        <v>619</v>
+        <v>618</v>
       </c>
       <c r="B127" s="52" t="s">
-        <v>494</v>
+        <v>493</v>
       </c>
       <c r="C127" s="52"/>
       <c r="D127" s="41"/>
@@ -40321,21 +40320,21 @@
     </row>
     <row r="128" ht="15.75" customHeight="1">
       <c r="A128" s="50" t="s">
-        <v>620</v>
+        <v>619</v>
       </c>
       <c r="B128" s="52" t="s">
-        <v>494</v>
+        <v>493</v>
       </c>
       <c r="C128" s="52" t="s">
-        <v>494</v>
+        <v>493</v>
       </c>
       <c r="D128" s="41"/>
       <c r="E128" s="41"/>
       <c r="F128" s="52" t="s">
-        <v>494</v>
+        <v>493</v>
       </c>
       <c r="G128" s="52" t="s">
-        <v>494</v>
+        <v>493</v>
       </c>
       <c r="H128" s="41"/>
       <c r="I128" s="41"/>
@@ -40359,14 +40358,14 @@
     </row>
     <row r="129" ht="15.75" customHeight="1">
       <c r="A129" s="50" t="s">
-        <v>621</v>
+        <v>620</v>
       </c>
       <c r="B129" s="52" t="s">
-        <v>494</v>
+        <v>493</v>
       </c>
       <c r="C129" s="42"/>
       <c r="D129" s="52" t="s">
-        <v>494</v>
+        <v>493</v>
       </c>
       <c r="E129" s="41"/>
       <c r="F129" s="41"/>
@@ -40393,10 +40392,10 @@
     </row>
     <row r="130" ht="15.75" customHeight="1">
       <c r="A130" s="50" t="s">
-        <v>622</v>
+        <v>621</v>
       </c>
       <c r="B130" s="52" t="s">
-        <v>494</v>
+        <v>493</v>
       </c>
       <c r="C130" s="41"/>
       <c r="D130" s="41"/>
@@ -40425,16 +40424,16 @@
     </row>
     <row r="131" ht="15.75" customHeight="1">
       <c r="A131" s="50" t="s">
-        <v>623</v>
+        <v>622</v>
       </c>
       <c r="B131" s="52" t="s">
-        <v>494</v>
+        <v>493</v>
       </c>
       <c r="C131" s="52" t="s">
-        <v>494</v>
+        <v>493</v>
       </c>
       <c r="D131" s="52" t="s">
-        <v>494</v>
+        <v>493</v>
       </c>
       <c r="E131" s="41"/>
       <c r="F131" s="41"/>
@@ -40461,14 +40460,14 @@
     </row>
     <row r="132" ht="15.75" customHeight="1">
       <c r="A132" s="50" t="s">
-        <v>624</v>
+        <v>623</v>
       </c>
       <c r="B132" s="52" t="s">
-        <v>494</v>
+        <v>493</v>
       </c>
       <c r="C132" s="42"/>
       <c r="D132" s="52" t="s">
-        <v>494</v>
+        <v>493</v>
       </c>
       <c r="E132" s="41"/>
       <c r="F132" s="41"/>
@@ -40495,16 +40494,16 @@
     </row>
     <row r="133" ht="15.75" customHeight="1">
       <c r="A133" s="50" t="s">
-        <v>625</v>
+        <v>624</v>
       </c>
       <c r="B133" s="52" t="s">
-        <v>494</v>
+        <v>493</v>
       </c>
       <c r="C133" s="52" t="s">
-        <v>494</v>
+        <v>493</v>
       </c>
       <c r="D133" s="52" t="s">
-        <v>494</v>
+        <v>493</v>
       </c>
       <c r="E133" s="41"/>
       <c r="F133" s="41"/>
@@ -40531,10 +40530,10 @@
     </row>
     <row r="134" ht="15.75" customHeight="1">
       <c r="A134" s="50" t="s">
-        <v>626</v>
+        <v>625</v>
       </c>
       <c r="B134" s="52" t="s">
-        <v>494</v>
+        <v>493</v>
       </c>
       <c r="C134" s="41"/>
       <c r="D134" s="41"/>
@@ -40563,17 +40562,17 @@
     </row>
     <row r="135" ht="15.75" customHeight="1">
       <c r="A135" s="50" t="s">
-        <v>627</v>
+        <v>626</v>
       </c>
       <c r="B135" s="52" t="s">
-        <v>494</v>
+        <v>493</v>
       </c>
       <c r="C135" s="41"/>
       <c r="D135" s="41"/>
       <c r="E135" s="41"/>
       <c r="F135" s="41"/>
       <c r="G135" s="52" t="s">
-        <v>494</v>
+        <v>493</v>
       </c>
       <c r="H135" s="41"/>
       <c r="I135" s="41"/>
@@ -40597,17 +40596,17 @@
     </row>
     <row r="136" ht="15.75" customHeight="1">
       <c r="A136" s="50" t="s">
-        <v>628</v>
+        <v>627</v>
       </c>
       <c r="B136" s="52" t="s">
-        <v>494</v>
+        <v>493</v>
       </c>
       <c r="C136" s="42"/>
       <c r="D136" s="42"/>
       <c r="E136" s="41"/>
       <c r="F136" s="41"/>
       <c r="G136" s="52" t="s">
-        <v>494</v>
+        <v>493</v>
       </c>
       <c r="H136" s="41"/>
       <c r="I136" s="41"/>
@@ -40631,17 +40630,17 @@
     </row>
     <row r="137" ht="15.75" customHeight="1">
       <c r="A137" s="50" t="s">
-        <v>629</v>
+        <v>628</v>
       </c>
       <c r="B137" s="52" t="s">
-        <v>494</v>
+        <v>493</v>
       </c>
       <c r="C137" s="41"/>
       <c r="D137" s="41"/>
       <c r="E137" s="41"/>
       <c r="F137" s="41"/>
       <c r="G137" s="52" t="s">
-        <v>494</v>
+        <v>493</v>
       </c>
       <c r="H137" s="41"/>
       <c r="I137" s="41"/>
@@ -40665,17 +40664,17 @@
     </row>
     <row r="138" ht="15.75" customHeight="1">
       <c r="A138" s="50" t="s">
-        <v>630</v>
+        <v>629</v>
       </c>
       <c r="B138" s="52" t="s">
-        <v>494</v>
+        <v>493</v>
       </c>
       <c r="C138" s="41"/>
       <c r="D138" s="41"/>
       <c r="E138" s="41"/>
       <c r="F138" s="41"/>
       <c r="G138" s="52" t="s">
-        <v>494</v>
+        <v>493</v>
       </c>
       <c r="H138" s="41"/>
       <c r="I138" s="41"/>
@@ -40699,17 +40698,17 @@
     </row>
     <row r="139" ht="15.75" customHeight="1">
       <c r="A139" s="50" t="s">
-        <v>631</v>
+        <v>630</v>
       </c>
       <c r="B139" s="52" t="s">
-        <v>494</v>
+        <v>493</v>
       </c>
       <c r="C139" s="41"/>
       <c r="D139" s="41"/>
       <c r="E139" s="41"/>
       <c r="F139" s="41"/>
       <c r="G139" s="52" t="s">
-        <v>494</v>
+        <v>493</v>
       </c>
       <c r="H139" s="41"/>
       <c r="I139" s="41"/>
@@ -40733,10 +40732,10 @@
     </row>
     <row r="140" ht="15.75" customHeight="1">
       <c r="A140" s="50" t="s">
-        <v>632</v>
+        <v>631</v>
       </c>
       <c r="B140" s="52" t="s">
-        <v>494</v>
+        <v>493</v>
       </c>
       <c r="C140" s="41"/>
       <c r="D140" s="41"/>
@@ -40765,10 +40764,10 @@
     </row>
     <row r="141" ht="15.75" customHeight="1">
       <c r="A141" s="50" t="s">
-        <v>633</v>
+        <v>632</v>
       </c>
       <c r="B141" s="52" t="s">
-        <v>494</v>
+        <v>493</v>
       </c>
       <c r="C141" s="41"/>
       <c r="D141" s="41"/>
@@ -40797,17 +40796,17 @@
     </row>
     <row r="142" ht="15.75" customHeight="1">
       <c r="A142" s="50" t="s">
-        <v>634</v>
+        <v>633</v>
       </c>
       <c r="B142" s="52" t="s">
-        <v>494</v>
+        <v>493</v>
       </c>
       <c r="C142" s="41"/>
       <c r="D142" s="41"/>
       <c r="E142" s="41"/>
       <c r="F142" s="41"/>
       <c r="G142" s="52" t="s">
-        <v>494</v>
+        <v>493</v>
       </c>
       <c r="H142" s="41"/>
       <c r="I142" s="41"/>
@@ -40831,10 +40830,10 @@
     </row>
     <row r="143" ht="15.75" customHeight="1">
       <c r="A143" s="50" t="s">
-        <v>635</v>
+        <v>634</v>
       </c>
       <c r="B143" s="52" t="s">
-        <v>494</v>
+        <v>493</v>
       </c>
       <c r="C143" s="41"/>
       <c r="D143" s="41"/>
@@ -40863,10 +40862,10 @@
     </row>
     <row r="144" ht="15.75" customHeight="1">
       <c r="A144" s="50" t="s">
-        <v>636</v>
+        <v>635</v>
       </c>
       <c r="B144" s="52" t="s">
-        <v>494</v>
+        <v>493</v>
       </c>
       <c r="C144" s="42"/>
       <c r="D144" s="41"/>
@@ -40895,10 +40894,10 @@
     </row>
     <row r="145" ht="15.75" customHeight="1">
       <c r="A145" s="50" t="s">
-        <v>637</v>
+        <v>636</v>
       </c>
       <c r="B145" s="52" t="s">
-        <v>494</v>
+        <v>493</v>
       </c>
       <c r="C145" s="41"/>
       <c r="D145" s="41"/>
@@ -40927,10 +40926,10 @@
     </row>
     <row r="146" ht="15.75" customHeight="1">
       <c r="A146" s="55" t="s">
-        <v>638</v>
+        <v>637</v>
       </c>
       <c r="B146" s="52" t="s">
-        <v>494</v>
+        <v>493</v>
       </c>
       <c r="C146" s="41"/>
       <c r="D146" s="41"/>
@@ -40959,10 +40958,10 @@
     </row>
     <row r="147" ht="15.75" customHeight="1">
       <c r="A147" s="55" t="s">
-        <v>639</v>
+        <v>638</v>
       </c>
       <c r="B147" s="52" t="s">
-        <v>494</v>
+        <v>493</v>
       </c>
       <c r="C147" s="41"/>
       <c r="D147" s="41"/>
@@ -40991,10 +40990,10 @@
     </row>
     <row r="148" ht="15.75" customHeight="1">
       <c r="A148" s="55" t="s">
-        <v>640</v>
+        <v>639</v>
       </c>
       <c r="B148" s="52" t="s">
-        <v>494</v>
+        <v>493</v>
       </c>
       <c r="C148" s="41"/>
       <c r="D148" s="41"/>
@@ -41023,14 +41022,14 @@
     </row>
     <row r="149" ht="15.75" customHeight="1">
       <c r="A149" s="55" t="s">
-        <v>641</v>
+        <v>640</v>
       </c>
       <c r="B149" s="52" t="s">
-        <v>494</v>
+        <v>493</v>
       </c>
       <c r="C149" s="41"/>
       <c r="D149" s="52" t="s">
-        <v>494</v>
+        <v>493</v>
       </c>
       <c r="E149" s="41"/>
       <c r="F149" s="41"/>
@@ -41057,10 +41056,10 @@
     </row>
     <row r="150" ht="15.75" customHeight="1">
       <c r="A150" s="55" t="s">
-        <v>642</v>
+        <v>641</v>
       </c>
       <c r="B150" s="52" t="s">
-        <v>494</v>
+        <v>493</v>
       </c>
       <c r="C150" s="41"/>
       <c r="D150" s="41"/>
@@ -41089,10 +41088,10 @@
     </row>
     <row r="151" ht="15.75" customHeight="1">
       <c r="A151" s="55" t="s">
-        <v>643</v>
+        <v>642</v>
       </c>
       <c r="B151" s="52" t="s">
-        <v>494</v>
+        <v>493</v>
       </c>
       <c r="C151" s="41"/>
       <c r="D151" s="41"/>
@@ -41121,17 +41120,17 @@
     </row>
     <row r="152" ht="15.75" customHeight="1">
       <c r="A152" s="55" t="s">
-        <v>644</v>
+        <v>643</v>
       </c>
       <c r="B152" s="52" t="s">
-        <v>494</v>
+        <v>493</v>
       </c>
       <c r="C152" s="41"/>
       <c r="D152" s="41"/>
       <c r="E152" s="41"/>
       <c r="F152" s="41"/>
       <c r="G152" s="52" t="s">
-        <v>494</v>
+        <v>493</v>
       </c>
       <c r="H152" s="55"/>
       <c r="I152" s="55"/>
@@ -41155,17 +41154,17 @@
     </row>
     <row r="153" ht="15.75" customHeight="1">
       <c r="A153" s="55" t="s">
-        <v>645</v>
+        <v>644</v>
       </c>
       <c r="B153" s="52" t="s">
-        <v>494</v>
+        <v>493</v>
       </c>
       <c r="C153" s="41"/>
       <c r="D153" s="41"/>
       <c r="E153" s="41"/>
       <c r="F153" s="41"/>
       <c r="G153" s="52" t="s">
-        <v>494</v>
+        <v>493</v>
       </c>
       <c r="H153" s="55"/>
       <c r="I153" s="55"/>
@@ -41189,21 +41188,21 @@
     </row>
     <row r="154" ht="15.75" customHeight="1">
       <c r="A154" s="55" t="s">
-        <v>646</v>
+        <v>645</v>
       </c>
       <c r="B154" s="52" t="s">
-        <v>494</v>
+        <v>493</v>
       </c>
       <c r="C154" s="52" t="s">
-        <v>494</v>
+        <v>493</v>
       </c>
       <c r="D154" s="41"/>
       <c r="E154" s="52" t="s">
-        <v>494</v>
+        <v>493</v>
       </c>
       <c r="F154" s="41"/>
       <c r="G154" s="52" t="s">
-        <v>494</v>
+        <v>493</v>
       </c>
       <c r="H154" s="55"/>
       <c r="I154" s="55"/>
@@ -41227,19 +41226,19 @@
     </row>
     <row r="155" ht="15.75" customHeight="1">
       <c r="A155" s="55" t="s">
-        <v>647</v>
+        <v>646</v>
       </c>
       <c r="B155" s="52" t="s">
-        <v>494</v>
+        <v>493</v>
       </c>
       <c r="C155" s="52" t="s">
-        <v>494</v>
+        <v>493</v>
       </c>
       <c r="D155" s="41"/>
       <c r="E155" s="41"/>
       <c r="F155" s="41"/>
       <c r="G155" s="52" t="s">
-        <v>494</v>
+        <v>493</v>
       </c>
       <c r="H155" s="55"/>
       <c r="I155" s="55"/>
@@ -41263,17 +41262,17 @@
     </row>
     <row r="156" ht="15.75" customHeight="1">
       <c r="A156" s="55" t="s">
-        <v>648</v>
+        <v>647</v>
       </c>
       <c r="B156" s="52" t="s">
-        <v>494</v>
+        <v>493</v>
       </c>
       <c r="C156" s="41"/>
       <c r="D156" s="41"/>
       <c r="E156" s="41"/>
       <c r="F156" s="41"/>
       <c r="G156" s="52" t="s">
-        <v>494</v>
+        <v>493</v>
       </c>
       <c r="H156" s="55"/>
       <c r="I156" s="55"/>
@@ -41297,17 +41296,17 @@
     </row>
     <row r="157" ht="15.75" customHeight="1">
       <c r="A157" s="55" t="s">
-        <v>649</v>
+        <v>648</v>
       </c>
       <c r="B157" s="52" t="s">
-        <v>494</v>
+        <v>493</v>
       </c>
       <c r="C157" s="41"/>
       <c r="D157" s="41"/>
       <c r="E157" s="41"/>
       <c r="F157" s="41"/>
       <c r="G157" s="52" t="s">
-        <v>494</v>
+        <v>493</v>
       </c>
       <c r="H157" s="55"/>
       <c r="I157" s="55"/>
@@ -41331,19 +41330,19 @@
     </row>
     <row r="158" ht="15.75" customHeight="1">
       <c r="A158" s="55" t="s">
-        <v>650</v>
+        <v>649</v>
       </c>
       <c r="B158" s="52" t="s">
-        <v>494</v>
+        <v>493</v>
       </c>
       <c r="C158" s="52" t="s">
-        <v>494</v>
+        <v>493</v>
       </c>
       <c r="D158" s="41"/>
       <c r="E158" s="41"/>
       <c r="F158" s="41"/>
       <c r="G158" s="52" t="s">
-        <v>494</v>
+        <v>493</v>
       </c>
       <c r="H158" s="55"/>
       <c r="I158" s="55"/>
@@ -41367,17 +41366,17 @@
     </row>
     <row r="159" ht="15.75" customHeight="1">
       <c r="A159" s="55" t="s">
-        <v>651</v>
+        <v>650</v>
       </c>
       <c r="B159" s="52" t="s">
-        <v>494</v>
+        <v>493</v>
       </c>
       <c r="C159" s="41"/>
       <c r="D159" s="41"/>
       <c r="E159" s="41"/>
       <c r="F159" s="41"/>
       <c r="G159" s="52" t="s">
-        <v>494</v>
+        <v>493</v>
       </c>
       <c r="H159" s="55"/>
       <c r="I159" s="55"/>
@@ -41401,19 +41400,19 @@
     </row>
     <row r="160" ht="15.75" customHeight="1">
       <c r="A160" s="55" t="s">
-        <v>652</v>
+        <v>651</v>
       </c>
       <c r="B160" s="52" t="s">
-        <v>494</v>
+        <v>493</v>
       </c>
       <c r="C160" s="52" t="s">
-        <v>494</v>
+        <v>493</v>
       </c>
       <c r="D160" s="41"/>
       <c r="E160" s="41"/>
       <c r="F160" s="41"/>
       <c r="G160" s="52" t="s">
-        <v>494</v>
+        <v>493</v>
       </c>
       <c r="H160" s="55"/>
       <c r="I160" s="55"/>
@@ -41437,17 +41436,17 @@
     </row>
     <row r="161" ht="15.75" customHeight="1">
       <c r="A161" s="55" t="s">
-        <v>653</v>
+        <v>652</v>
       </c>
       <c r="B161" s="52" t="s">
-        <v>494</v>
+        <v>493</v>
       </c>
       <c r="C161" s="41"/>
       <c r="D161" s="41"/>
       <c r="E161" s="41"/>
       <c r="F161" s="41"/>
       <c r="G161" s="52" t="s">
-        <v>494</v>
+        <v>493</v>
       </c>
       <c r="H161" s="55"/>
       <c r="I161" s="55"/>
@@ -41471,14 +41470,14 @@
     </row>
     <row r="162" ht="15.75" customHeight="1">
       <c r="A162" s="55" t="s">
-        <v>654</v>
+        <v>653</v>
       </c>
       <c r="B162" s="52" t="s">
-        <v>494</v>
+        <v>493</v>
       </c>
       <c r="C162" s="41"/>
       <c r="D162" s="52" t="s">
-        <v>494</v>
+        <v>493</v>
       </c>
       <c r="E162" s="41"/>
       <c r="F162" s="41"/>
@@ -41505,21 +41504,21 @@
     </row>
     <row r="163" ht="15.75" customHeight="1">
       <c r="A163" s="55" t="s">
-        <v>655</v>
+        <v>654</v>
       </c>
       <c r="B163" s="52" t="s">
-        <v>494</v>
+        <v>493</v>
       </c>
       <c r="C163" s="52" t="s">
-        <v>494</v>
+        <v>493</v>
       </c>
       <c r="D163" s="52" t="s">
-        <v>494</v>
+        <v>493</v>
       </c>
       <c r="E163" s="41"/>
       <c r="F163" s="41"/>
       <c r="G163" s="52" t="s">
-        <v>494</v>
+        <v>493</v>
       </c>
       <c r="H163" s="55"/>
       <c r="I163" s="55"/>
@@ -41543,10 +41542,10 @@
     </row>
     <row r="164" ht="15.75" customHeight="1">
       <c r="A164" s="55" t="s">
-        <v>656</v>
+        <v>655</v>
       </c>
       <c r="B164" s="52" t="s">
-        <v>494</v>
+        <v>493</v>
       </c>
       <c r="C164" s="41"/>
       <c r="D164" s="41"/>
@@ -41575,17 +41574,17 @@
     </row>
     <row r="165" ht="15.75" customHeight="1">
       <c r="A165" s="55" t="s">
-        <v>657</v>
+        <v>656</v>
       </c>
       <c r="B165" s="52" t="s">
-        <v>494</v>
+        <v>493</v>
       </c>
       <c r="C165" s="41"/>
       <c r="D165" s="41"/>
       <c r="E165" s="41"/>
       <c r="F165" s="41"/>
       <c r="G165" s="52" t="s">
-        <v>494</v>
+        <v>493</v>
       </c>
       <c r="H165" s="55"/>
       <c r="I165" s="55"/>
@@ -41609,19 +41608,19 @@
     </row>
     <row r="166" ht="15.75" customHeight="1">
       <c r="A166" s="55" t="s">
-        <v>658</v>
+        <v>657</v>
       </c>
       <c r="B166" s="52" t="s">
-        <v>494</v>
+        <v>493</v>
       </c>
       <c r="C166" s="52" t="s">
-        <v>494</v>
+        <v>493</v>
       </c>
       <c r="D166" s="41"/>
       <c r="E166" s="41"/>
       <c r="F166" s="41"/>
       <c r="G166" s="52" t="s">
-        <v>494</v>
+        <v>493</v>
       </c>
       <c r="H166" s="55"/>
       <c r="I166" s="55"/>
@@ -41645,19 +41644,19 @@
     </row>
     <row r="167" ht="15.75" customHeight="1">
       <c r="A167" s="55" t="s">
-        <v>659</v>
+        <v>658</v>
       </c>
       <c r="B167" s="52" t="s">
-        <v>494</v>
+        <v>493</v>
       </c>
       <c r="C167" s="52" t="s">
-        <v>494</v>
+        <v>493</v>
       </c>
       <c r="D167" s="41"/>
       <c r="E167" s="41"/>
       <c r="F167" s="41"/>
       <c r="G167" s="52" t="s">
-        <v>494</v>
+        <v>493</v>
       </c>
       <c r="H167" s="55"/>
       <c r="I167" s="55"/>
@@ -41681,13 +41680,13 @@
     </row>
     <row r="168" ht="15.75" customHeight="1">
       <c r="A168" s="55" t="s">
-        <v>660</v>
+        <v>659</v>
       </c>
       <c r="B168" s="52" t="s">
-        <v>494</v>
+        <v>493</v>
       </c>
       <c r="C168" s="52" t="s">
-        <v>494</v>
+        <v>493</v>
       </c>
       <c r="D168" s="41"/>
       <c r="E168" s="41"/>
@@ -41715,13 +41714,13 @@
     </row>
     <row r="169" ht="15.75" customHeight="1">
       <c r="A169" s="55" t="s">
-        <v>661</v>
+        <v>660</v>
       </c>
       <c r="B169" s="52" t="s">
-        <v>494</v>
+        <v>493</v>
       </c>
       <c r="C169" s="52" t="s">
-        <v>494</v>
+        <v>493</v>
       </c>
       <c r="D169" s="41"/>
       <c r="E169" s="41"/>
@@ -41749,15 +41748,15 @@
     </row>
     <row r="170" ht="15.75" customHeight="1">
       <c r="A170" s="55" t="s">
-        <v>662</v>
+        <v>661</v>
       </c>
       <c r="B170" s="56"/>
       <c r="C170" s="52" t="s">
-        <v>494</v>
+        <v>493</v>
       </c>
       <c r="D170" s="41"/>
       <c r="E170" s="52" t="s">
-        <v>494</v>
+        <v>493</v>
       </c>
       <c r="F170" s="41"/>
       <c r="G170" s="41"/>
@@ -41783,17 +41782,17 @@
     </row>
     <row r="171" ht="15.75" customHeight="1">
       <c r="A171" s="55" t="s">
-        <v>663</v>
+        <v>662</v>
       </c>
       <c r="B171" s="52" t="s">
-        <v>494</v>
+        <v>493</v>
       </c>
       <c r="C171" s="41"/>
       <c r="D171" s="41"/>
       <c r="E171" s="41"/>
       <c r="F171" s="41"/>
       <c r="G171" s="52" t="s">
-        <v>494</v>
+        <v>493</v>
       </c>
       <c r="H171" s="55"/>
       <c r="I171" s="55"/>
@@ -41817,21 +41816,21 @@
     </row>
     <row r="172" ht="15.75" customHeight="1">
       <c r="A172" s="55" t="s">
-        <v>664</v>
+        <v>663</v>
       </c>
       <c r="B172" s="52" t="s">
-        <v>494</v>
+        <v>493</v>
       </c>
       <c r="C172" s="52" t="s">
-        <v>494</v>
+        <v>493</v>
       </c>
       <c r="D172" s="41"/>
       <c r="E172" s="52" t="s">
-        <v>494</v>
+        <v>493</v>
       </c>
       <c r="F172" s="41"/>
       <c r="G172" s="52" t="s">
-        <v>494</v>
+        <v>493</v>
       </c>
       <c r="H172" s="55"/>
       <c r="I172" s="55"/>
@@ -41855,10 +41854,10 @@
     </row>
     <row r="173" ht="15.75" customHeight="1">
       <c r="A173" s="55" t="s">
-        <v>665</v>
+        <v>664</v>
       </c>
       <c r="B173" s="52" t="s">
-        <v>494</v>
+        <v>493</v>
       </c>
       <c r="C173" s="41"/>
       <c r="D173" s="41"/>
@@ -41887,10 +41886,10 @@
     </row>
     <row r="174" ht="15.75" customHeight="1">
       <c r="A174" s="55" t="s">
-        <v>666</v>
+        <v>665</v>
       </c>
       <c r="B174" s="52" t="s">
-        <v>494</v>
+        <v>493</v>
       </c>
       <c r="C174" s="41"/>
       <c r="D174" s="41"/>
@@ -41919,17 +41918,17 @@
     </row>
     <row r="175" ht="15.75" customHeight="1">
       <c r="A175" s="55" t="s">
-        <v>667</v>
+        <v>666</v>
       </c>
       <c r="B175" s="52" t="s">
-        <v>494</v>
+        <v>493</v>
       </c>
       <c r="C175" s="41"/>
       <c r="D175" s="41"/>
       <c r="E175" s="41"/>
       <c r="F175" s="41"/>
       <c r="G175" s="52" t="s">
-        <v>494</v>
+        <v>493</v>
       </c>
       <c r="H175" s="55"/>
       <c r="I175" s="55"/>
@@ -41953,10 +41952,10 @@
     </row>
     <row r="176" ht="15.75" customHeight="1">
       <c r="A176" s="55" t="s">
-        <v>668</v>
+        <v>667</v>
       </c>
       <c r="B176" s="52" t="s">
-        <v>494</v>
+        <v>493</v>
       </c>
       <c r="C176" s="41"/>
       <c r="D176" s="41"/>
@@ -41985,17 +41984,17 @@
     </row>
     <row r="177" ht="15.75" customHeight="1">
       <c r="A177" s="55" t="s">
-        <v>669</v>
+        <v>668</v>
       </c>
       <c r="B177" s="52" t="s">
-        <v>494</v>
+        <v>493</v>
       </c>
       <c r="C177" s="41"/>
       <c r="D177" s="41"/>
       <c r="E177" s="41"/>
       <c r="F177" s="41"/>
       <c r="G177" s="52" t="s">
-        <v>494</v>
+        <v>493</v>
       </c>
       <c r="H177" s="55"/>
       <c r="I177" s="55"/>
@@ -42019,17 +42018,17 @@
     </row>
     <row r="178" ht="15.75" customHeight="1">
       <c r="A178" s="55" t="s">
-        <v>670</v>
+        <v>669</v>
       </c>
       <c r="B178" s="52" t="s">
-        <v>494</v>
+        <v>493</v>
       </c>
       <c r="C178" s="41"/>
       <c r="D178" s="41"/>
       <c r="E178" s="41"/>
       <c r="F178" s="41"/>
       <c r="G178" s="52" t="s">
-        <v>494</v>
+        <v>493</v>
       </c>
       <c r="H178" s="55"/>
       <c r="I178" s="55"/>
@@ -42053,17 +42052,17 @@
     </row>
     <row r="179" ht="15.75" customHeight="1">
       <c r="A179" s="55" t="s">
-        <v>671</v>
+        <v>670</v>
       </c>
       <c r="B179" s="52" t="s">
-        <v>494</v>
+        <v>493</v>
       </c>
       <c r="C179" s="41"/>
       <c r="D179" s="41"/>
       <c r="E179" s="41"/>
       <c r="F179" s="41"/>
       <c r="G179" s="52" t="s">
-        <v>494</v>
+        <v>493</v>
       </c>
       <c r="H179" s="55"/>
       <c r="I179" s="55"/>
@@ -42087,17 +42086,17 @@
     </row>
     <row r="180" ht="15.75" customHeight="1">
       <c r="A180" s="55" t="s">
-        <v>672</v>
+        <v>671</v>
       </c>
       <c r="B180" s="52" t="s">
-        <v>494</v>
+        <v>493</v>
       </c>
       <c r="C180" s="41"/>
       <c r="D180" s="41"/>
       <c r="E180" s="41"/>
       <c r="F180" s="41"/>
       <c r="G180" s="52" t="s">
-        <v>494</v>
+        <v>493</v>
       </c>
       <c r="H180" s="55"/>
       <c r="I180" s="55"/>
@@ -42121,17 +42120,17 @@
     </row>
     <row r="181" ht="15.75" customHeight="1">
       <c r="A181" s="55" t="s">
-        <v>673</v>
+        <v>672</v>
       </c>
       <c r="B181" s="52" t="s">
-        <v>494</v>
+        <v>493</v>
       </c>
       <c r="C181" s="41"/>
       <c r="D181" s="41"/>
       <c r="E181" s="41"/>
       <c r="F181" s="41"/>
       <c r="G181" s="52" t="s">
-        <v>494</v>
+        <v>493</v>
       </c>
       <c r="H181" s="55"/>
       <c r="I181" s="55"/>
@@ -42155,10 +42154,10 @@
     </row>
     <row r="182" ht="15.75" customHeight="1">
       <c r="A182" s="55" t="s">
-        <v>674</v>
+        <v>673</v>
       </c>
       <c r="B182" s="52" t="s">
-        <v>494</v>
+        <v>493</v>
       </c>
       <c r="C182" s="41"/>
       <c r="D182" s="41"/>
@@ -42187,10 +42186,10 @@
     </row>
     <row r="183" ht="15.75" customHeight="1">
       <c r="A183" s="55" t="s">
-        <v>675</v>
+        <v>674</v>
       </c>
       <c r="B183" s="52" t="s">
-        <v>494</v>
+        <v>493</v>
       </c>
       <c r="C183" s="41"/>
       <c r="D183" s="41"/>
@@ -42219,17 +42218,17 @@
     </row>
     <row r="184" ht="15.75" customHeight="1">
       <c r="A184" s="55" t="s">
-        <v>676</v>
+        <v>675</v>
       </c>
       <c r="B184" s="52" t="s">
-        <v>494</v>
+        <v>493</v>
       </c>
       <c r="C184" s="41"/>
       <c r="D184" s="41"/>
       <c r="E184" s="41"/>
       <c r="F184" s="41"/>
       <c r="G184" s="52" t="s">
-        <v>494</v>
+        <v>493</v>
       </c>
       <c r="H184" s="55"/>
       <c r="I184" s="55"/>
@@ -42253,10 +42252,10 @@
     </row>
     <row r="185" ht="15.75" customHeight="1">
       <c r="A185" s="55" t="s">
-        <v>677</v>
+        <v>676</v>
       </c>
       <c r="B185" s="52" t="s">
-        <v>494</v>
+        <v>493</v>
       </c>
       <c r="C185" s="41"/>
       <c r="D185" s="41"/>
@@ -42285,16 +42284,16 @@
     </row>
     <row r="186" ht="15.75" customHeight="1">
       <c r="A186" s="55" t="s">
-        <v>678</v>
+        <v>677</v>
       </c>
       <c r="B186" s="52" t="s">
-        <v>494</v>
+        <v>493</v>
       </c>
       <c r="C186" s="52" t="s">
-        <v>494</v>
+        <v>493</v>
       </c>
       <c r="D186" s="52" t="s">
-        <v>494</v>
+        <v>493</v>
       </c>
       <c r="E186" s="41"/>
       <c r="F186" s="41"/>
@@ -42321,14 +42320,14 @@
     </row>
     <row r="187" ht="15.75" customHeight="1">
       <c r="A187" s="55" t="s">
-        <v>679</v>
+        <v>678</v>
       </c>
       <c r="B187" s="52" t="s">
-        <v>494</v>
+        <v>493</v>
       </c>
       <c r="C187" s="41"/>
       <c r="D187" s="52" t="s">
-        <v>494</v>
+        <v>493</v>
       </c>
       <c r="E187" s="41"/>
       <c r="F187" s="41"/>
@@ -42355,10 +42354,10 @@
     </row>
     <row r="188" ht="15.75" customHeight="1">
       <c r="A188" s="55" t="s">
-        <v>680</v>
+        <v>679</v>
       </c>
       <c r="B188" s="52" t="s">
-        <v>494</v>
+        <v>493</v>
       </c>
       <c r="C188" s="41"/>
       <c r="D188" s="41"/>
@@ -42387,16 +42386,16 @@
     </row>
     <row r="189" ht="15.75" customHeight="1">
       <c r="A189" s="55" t="s">
-        <v>681</v>
+        <v>680</v>
       </c>
       <c r="B189" s="52" t="s">
-        <v>494</v>
+        <v>493</v>
       </c>
       <c r="C189" s="52" t="s">
-        <v>494</v>
+        <v>493</v>
       </c>
       <c r="D189" s="52" t="s">
-        <v>494</v>
+        <v>493</v>
       </c>
       <c r="E189" s="41"/>
       <c r="F189" s="41"/>
@@ -42423,21 +42422,21 @@
     </row>
     <row r="190" ht="15.75" customHeight="1">
       <c r="A190" s="55" t="s">
-        <v>682</v>
+        <v>681</v>
       </c>
       <c r="B190" s="52" t="s">
-        <v>494</v>
+        <v>493</v>
       </c>
       <c r="C190" s="52" t="s">
-        <v>494</v>
+        <v>493</v>
       </c>
       <c r="D190" s="52" t="s">
-        <v>494</v>
+        <v>493</v>
       </c>
       <c r="E190" s="41"/>
       <c r="F190" s="41"/>
       <c r="G190" s="52" t="s">
-        <v>494</v>
+        <v>493</v>
       </c>
       <c r="H190" s="55"/>
       <c r="I190" s="55"/>
@@ -42461,10 +42460,10 @@
     </row>
     <row r="191" ht="15.75" customHeight="1">
       <c r="A191" s="55" t="s">
-        <v>683</v>
+        <v>682</v>
       </c>
       <c r="B191" s="52" t="s">
-        <v>494</v>
+        <v>493</v>
       </c>
       <c r="C191" s="56"/>
       <c r="D191" s="56"/>
@@ -42493,17 +42492,17 @@
     </row>
     <row r="192" ht="15.75" customHeight="1">
       <c r="A192" s="55" t="s">
-        <v>684</v>
+        <v>683</v>
       </c>
       <c r="B192" s="52" t="s">
-        <v>494</v>
+        <v>493</v>
       </c>
       <c r="C192" s="55"/>
       <c r="D192" s="41"/>
       <c r="E192" s="41"/>
       <c r="F192" s="41"/>
       <c r="G192" s="52" t="s">
-        <v>494</v>
+        <v>493</v>
       </c>
       <c r="H192" s="55"/>
       <c r="I192" s="55"/>
@@ -42527,17 +42526,17 @@
     </row>
     <row r="193" ht="15.75" customHeight="1">
       <c r="A193" s="55" t="s">
-        <v>685</v>
+        <v>684</v>
       </c>
       <c r="B193" s="52" t="s">
-        <v>494</v>
+        <v>493</v>
       </c>
       <c r="C193" s="41"/>
       <c r="D193" s="41"/>
       <c r="E193" s="41"/>
       <c r="F193" s="41"/>
       <c r="G193" s="52" t="s">
-        <v>494</v>
+        <v>493</v>
       </c>
       <c r="H193" s="55"/>
       <c r="I193" s="55"/>
@@ -42561,17 +42560,17 @@
     </row>
     <row r="194" ht="15.75" customHeight="1">
       <c r="A194" s="55" t="s">
-        <v>686</v>
+        <v>685</v>
       </c>
       <c r="B194" s="52" t="s">
-        <v>494</v>
+        <v>493</v>
       </c>
       <c r="C194" s="41"/>
       <c r="D194" s="41"/>
       <c r="E194" s="41"/>
       <c r="F194" s="41"/>
       <c r="G194" s="52" t="s">
-        <v>494</v>
+        <v>493</v>
       </c>
       <c r="H194" s="55"/>
       <c r="I194" s="55"/>

</xml_diff>